<commit_message>
set up double type permanently
added a line at the beginning of master to set up the var type to be double permanently.
removed all double definitions within the rest of the code. Thanks to @MayaGoldman!
</commit_message>
<xml_diff>
--- a/03.Tool/Example_FiscalSim.xlsx
+++ b/03.Tool/Example_FiscalSim.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7027" uniqueCount="1483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10333" uniqueCount="1483">
   <si>
     <t>Bracket</t>
   </si>
@@ -15551,25 +15551,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="87">
-        <v>34626.576694199313</v>
+        <v>34626.576666144567</v>
       </c>
       <c r="C2" s="87">
-        <v>34742.247068984019</v>
+        <v>34742.247079590714</v>
       </c>
       <c r="D2" s="87">
-        <v>28461.362606342478</v>
+        <v>28461.362600937126</v>
       </c>
       <c r="E2" s="87">
-        <v>40725.268789028414</v>
+        <v>40725.26874993628</v>
       </c>
       <c r="F2" s="87">
-        <v>34560.054687575735</v>
+        <v>34560.054684728835</v>
       </c>
       <c r="G2" s="87">
-        <v>32072.252118168544</v>
+        <v>32072.25213091361</v>
       </c>
       <c r="H2" s="87">
-        <v>34884.752098017874</v>
+        <v>34884.752130913614</v>
       </c>
       <c r="I2" s="87">
         <v>-4061.5879684336987</v>
@@ -15587,7 +15587,7 @@
         <v>-3360.1577448095431</v>
       </c>
       <c r="N2" s="87">
-        <v>872.35519157940223</v>
+        <v>872.35519099431519</v>
       </c>
       <c r="O2" s="87">
         <v>1312.5</v>
@@ -15638,10 +15638,10 @@
         <v>-3301.1215805508518</v>
       </c>
       <c r="AE2" s="64">
-        <v>-59.036164258691223</v>
+        <v>-59.036164258691215</v>
       </c>
       <c r="AF2" s="64">
-        <v>872.35519157940223</v>
+        <v>872.35519099431519</v>
       </c>
       <c r="AG2" s="64">
         <v>825</v>
@@ -15864,25 +15864,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="64">
-        <v>202.23070414028234</v>
+        <v>202.2307041744391</v>
       </c>
       <c r="C5" s="64">
-        <v>1622.4209087922775</v>
+        <v>1622.4209093790053</v>
       </c>
       <c r="D5" s="64">
-        <v>201.25996113351502</v>
+        <v>201.25996113664488</v>
       </c>
       <c r="E5" s="64">
-        <v>1927.1375067061351</v>
+        <v>1927.137506984383</v>
       </c>
       <c r="F5" s="64">
-        <v>1926.1667640799774</v>
+        <v>1926.1667639465888</v>
       </c>
       <c r="G5" s="64">
-        <v>1753.181366671861</v>
+        <v>1753.1813653725301</v>
       </c>
       <c r="H5" s="64">
-        <v>2046.3024947712013</v>
+        <v>2046.3024927733568</v>
       </c>
       <c r="I5" s="64">
         <v>-0.94601628107910674</v>
@@ -15900,7 +15900,7 @@
         <v>-244.16186146292813</v>
       </c>
       <c r="N5" s="64">
-        <v>71.176462781010798</v>
+        <v>71.176462888869267</v>
       </c>
       <c r="O5" s="64">
         <v>251.73904696832213</v>
@@ -15954,7 +15954,7 @@
         <v>-2.1713410367311874</v>
       </c>
       <c r="AF5" s="64">
-        <v>71.176462781010798</v>
+        <v>71.176462888869267</v>
       </c>
       <c r="AG5" s="64">
         <v>192.84349644442747</v>
@@ -15994,25 +15994,25 @@
         <v>2</v>
       </c>
       <c r="B6" s="64">
-        <v>723.72293336578196</v>
+        <v>723.72293256850935</v>
       </c>
       <c r="C6" s="64">
-        <v>1429.5882757622785</v>
+        <v>1429.5882750326766</v>
       </c>
       <c r="D6" s="64">
-        <v>708.51535089657136</v>
+        <v>708.51535054605063</v>
       </c>
       <c r="E6" s="64">
-        <v>1808.4035991896617</v>
+        <v>1808.403601048328</v>
       </c>
       <c r="F6" s="64">
-        <v>1793.1960187236841</v>
+        <v>1793.1960190258692</v>
       </c>
       <c r="G6" s="64">
-        <v>1667.7427480499211</v>
+        <v>1667.7427495874608</v>
       </c>
       <c r="H6" s="64">
-        <v>1960.0890615482519</v>
+        <v>1960.0890616219558</v>
       </c>
       <c r="I6" s="64">
         <v>-13.509524141361005</v>
@@ -16030,7 +16030,7 @@
         <v>-200.91087256420764</v>
       </c>
       <c r="N6" s="64">
-        <v>75.457603154096631</v>
+        <v>75.457603125799267</v>
       </c>
       <c r="O6" s="64">
         <v>180.71042964292116</v>
@@ -16072,7 +16072,7 @@
         <v>102.35091051285275</v>
       </c>
       <c r="AB6" s="64">
-        <v>202.01969463012031</v>
+        <v>202.01969463012034</v>
       </c>
       <c r="AC6" s="64">
         <v>26.697186804669059</v>
@@ -16084,7 +16084,7 @@
         <v>-2.6471003754914588</v>
       </c>
       <c r="AF6" s="64">
-        <v>75.457603154096631</v>
+        <v>75.457603125799267</v>
       </c>
       <c r="AG6" s="64">
         <v>131.6529267776971</v>
@@ -16124,25 +16124,25 @@
         <v>3</v>
       </c>
       <c r="B7" s="64">
-        <v>1317.0785453541848</v>
+        <v>1317.0785457704399</v>
       </c>
       <c r="C7" s="64">
-        <v>1643.2727825409524</v>
+        <v>1643.2727821589217</v>
       </c>
       <c r="D7" s="64">
-        <v>1241.7188369829628</v>
+        <v>1241.7188372235157</v>
       </c>
       <c r="E7" s="64">
-        <v>1958.1574085376237</v>
+        <v>1958.1574061530102</v>
       </c>
       <c r="F7" s="64">
-        <v>1882.7976980200572</v>
+        <v>1882.7976976060861</v>
       </c>
       <c r="G7" s="64">
-        <v>1760.4003760595197</v>
+        <v>1760.400372659082</v>
       </c>
       <c r="H7" s="64">
-        <v>2016.3859967311907</v>
+        <v>2016.386000056207</v>
       </c>
       <c r="I7" s="64">
         <v>-61.357439456544945</v>
@@ -16160,7 +16160,7 @@
         <v>-207.71731629546278</v>
       </c>
       <c r="N7" s="64">
-        <v>85.319991271547508</v>
+        <v>85.319991348458771</v>
       </c>
       <c r="O7" s="64">
         <v>123.28912608895374</v>
@@ -16202,7 +16202,7 @@
         <v>132.85961948036345</v>
       </c>
       <c r="AB7" s="64">
-        <v>43.772284843047323</v>
+        <v>43.772284843047316</v>
       </c>
       <c r="AC7" s="64">
         <v>20.584079968696734</v>
@@ -16211,10 +16211,10 @@
         <v>-205.31643736506709</v>
       </c>
       <c r="AE7" s="64">
-        <v>-2.4008789303956903</v>
+        <v>-2.4008789303956894</v>
       </c>
       <c r="AF7" s="64">
-        <v>85.319991271547508</v>
+        <v>85.319991348458771</v>
       </c>
       <c r="AG7" s="64">
         <v>79.634306410498709</v>
@@ -16254,25 +16254,25 @@
         <v>4</v>
       </c>
       <c r="B8" s="64">
-        <v>1856.4720415876127</v>
+        <v>1856.4720358119571</v>
       </c>
       <c r="C8" s="64">
-        <v>2015.967979963795</v>
+        <v>2015.9679783924366</v>
       </c>
       <c r="D8" s="64">
-        <v>1678.5539213111717</v>
+        <v>1678.5539212909553</v>
       </c>
       <c r="E8" s="64">
-        <v>2358.5607084851331</v>
+        <v>2358.5607030731285</v>
       </c>
       <c r="F8" s="64">
-        <v>2180.6425908253314</v>
+        <v>2180.6425885521271</v>
       </c>
       <c r="G8" s="64">
-        <v>2043.1964466242337</v>
+        <v>2043.1964508779306</v>
       </c>
       <c r="H8" s="64">
-        <v>2370.0170993854272</v>
+        <v>2370.0171042214029</v>
       </c>
       <c r="I8" s="64">
         <v>-133.52492174612155</v>
@@ -16290,7 +16290,7 @@
         <v>-222.93210943209294</v>
       </c>
       <c r="N8" s="64">
-        <v>85.485971832550931</v>
+        <v>85.485971757896749</v>
       </c>
       <c r="O8" s="64">
         <v>151.76127646965907</v>
@@ -16341,10 +16341,10 @@
         <v>-219.94344432662987</v>
       </c>
       <c r="AE8" s="64">
-        <v>-2.9886651054630589</v>
+        <v>-2.9886651054630584</v>
       </c>
       <c r="AF8" s="64">
-        <v>85.485971832550931</v>
+        <v>85.485971757896749</v>
       </c>
       <c r="AG8" s="64">
         <v>106.63939414586044</v>
@@ -16384,25 +16384,25 @@
         <v>5</v>
       </c>
       <c r="B9" s="64">
-        <v>2356.2046839050663</v>
+        <v>2356.2046889419216</v>
       </c>
       <c r="C9" s="64">
-        <v>2433.3226859596653</v>
+        <v>2433.3226874121256</v>
       </c>
       <c r="D9" s="64">
-        <v>2091.4814283678247</v>
+        <v>2091.4814259435484</v>
       </c>
       <c r="E9" s="64">
-        <v>2842.7704816783898</v>
+        <v>2842.7704808913036</v>
       </c>
       <c r="F9" s="64">
-        <v>2578.0472191367749</v>
+        <v>2578.0472178929299</v>
       </c>
       <c r="G9" s="64">
-        <v>2392.5662020889558</v>
+        <v>2392.5662022571441</v>
       </c>
       <c r="H9" s="64">
-        <v>2667.3594002002546</v>
+        <v>2667.3594001286533</v>
       </c>
       <c r="I9" s="64">
         <v>-192.29657594502629</v>
@@ -16420,7 +16420,7 @@
         <v>-272.44733957120559</v>
       </c>
       <c r="N9" s="64">
-        <v>86.966323997305437</v>
+        <v>86.966323935419823</v>
       </c>
       <c r="O9" s="64">
         <v>104.17281922168424</v>
@@ -16471,10 +16471,10 @@
         <v>-268.27496862542802</v>
       </c>
       <c r="AE9" s="64">
-        <v>-4.1723709457776028</v>
+        <v>-4.1723709457776019</v>
       </c>
       <c r="AF9" s="64">
-        <v>86.966323997305437</v>
+        <v>86.966323935419823</v>
       </c>
       <c r="AG9" s="64">
         <v>58.218166779389271</v>
@@ -16514,25 +16514,25 @@
         <v>6</v>
       </c>
       <c r="B10" s="64">
-        <v>2980.6606639895499</v>
+        <v>2980.6606644910712</v>
       </c>
       <c r="C10" s="64">
-        <v>2960.2102794073899</v>
+        <v>2960.210278352281</v>
       </c>
       <c r="D10" s="64">
-        <v>2589.5680840255172</v>
+        <v>2589.5680829890753</v>
       </c>
       <c r="E10" s="64">
-        <v>3384.5019184087455</v>
+        <v>3384.5019209289094</v>
       </c>
       <c r="F10" s="64">
-        <v>2993.4093403038455</v>
+        <v>2993.409339426913</v>
       </c>
       <c r="G10" s="64">
-        <v>2793.4060956044527</v>
+        <v>2793.4060895746406</v>
       </c>
       <c r="H10" s="64">
-        <v>3071.3763104159866</v>
+        <v>3071.3763074864278</v>
       </c>
       <c r="I10" s="64">
         <v>-272.80787195304993</v>
@@ -16550,7 +16550,7 @@
         <v>-291.91293832265802</v>
       </c>
       <c r="N10" s="64">
-        <v>91.909688539330048</v>
+        <v>91.909688470385944</v>
       </c>
       <c r="O10" s="64">
         <v>106.96250128969831</v>
@@ -16598,13 +16598,13 @@
         <v>11.350661428007504</v>
       </c>
       <c r="AD10" s="64">
-        <v>-287.04599185520027</v>
+        <v>-287.04599185520021</v>
       </c>
       <c r="AE10" s="64">
         <v>-4.8669464674577281</v>
       </c>
       <c r="AF10" s="64">
-        <v>91.909688539330048</v>
+        <v>91.909688470385944</v>
       </c>
       <c r="AG10" s="64">
         <v>62.568713166285619</v>
@@ -16644,25 +16644,25 @@
         <v>7</v>
       </c>
       <c r="B11" s="64">
-        <v>3665.044860056943</v>
+        <v>3665.0448557589307</v>
       </c>
       <c r="C11" s="64">
-        <v>3391.114427634699</v>
+        <v>3391.1144256215907</v>
       </c>
       <c r="D11" s="64">
-        <v>3031.8495685650046</v>
+        <v>3031.8495628637952</v>
       </c>
       <c r="E11" s="64">
-        <v>3983.1629097466994</v>
+        <v>3983.1629037445205</v>
       </c>
       <c r="F11" s="64">
-        <v>3349.9676177805804</v>
+        <v>3349.967610849385</v>
       </c>
       <c r="G11" s="64">
-        <v>3109.7528720227501</v>
+        <v>3109.7528780589014</v>
       </c>
       <c r="H11" s="64">
-        <v>3398.3901421811684</v>
+        <v>3398.3901424560145</v>
       </c>
       <c r="I11" s="64">
         <v>-440.82239638829861</v>
@@ -16680,7 +16680,7 @@
         <v>-332.35618541249272</v>
       </c>
       <c r="N11" s="64">
-        <v>92.141452868662398</v>
+        <v>92.141452622009027</v>
       </c>
       <c r="O11" s="64">
         <v>92.275493819450745</v>
@@ -16734,7 +16734,7 @@
         <v>-5.3965233600036768</v>
       </c>
       <c r="AF11" s="64">
-        <v>92.141452868662398</v>
+        <v>92.141452622009027</v>
       </c>
       <c r="AG11" s="64">
         <v>44.726368536714993</v>
@@ -16774,25 +16774,25 @@
         <v>8</v>
       </c>
       <c r="B12" s="64">
-        <v>4586.3162095128655</v>
+        <v>4586.3162020760983</v>
       </c>
       <c r="C12" s="64">
-        <v>4289.6049430081157</v>
+        <v>4289.6049454431868</v>
       </c>
       <c r="D12" s="64">
-        <v>3772.0476794943415</v>
+        <v>3772.0476774856425</v>
       </c>
       <c r="E12" s="64">
-        <v>4949.6086873391068</v>
+        <v>4949.6086792913784</v>
       </c>
       <c r="F12" s="64">
-        <v>4135.3401592172095</v>
+        <v>4135.3401547009216</v>
       </c>
       <c r="G12" s="64">
-        <v>3844.3237137674346</v>
+        <v>3844.3237084032844</v>
       </c>
       <c r="H12" s="64">
-        <v>4109.0916951937807</v>
+        <v>4109.0916989867374</v>
       </c>
       <c r="I12" s="64">
         <v>-542.10395597667821</v>
@@ -16810,7 +16810,7 @@
         <v>-385.91603740216641</v>
       </c>
       <c r="N12" s="64">
-        <v>94.899591210911808</v>
+        <v>94.899591104528767</v>
       </c>
       <c r="O12" s="64">
         <v>104.42431964175007</v>
@@ -16861,10 +16861,10 @@
         <v>-378.23533143712194</v>
       </c>
       <c r="AE12" s="64">
-        <v>-7.6807059650444671</v>
+        <v>-7.680705965044468</v>
       </c>
       <c r="AF12" s="64">
-        <v>94.899591210911808</v>
+        <v>94.899591104528767</v>
       </c>
       <c r="AG12" s="64">
         <v>57.729741520171679</v>
@@ -16904,25 +16904,25 @@
         <v>9</v>
       </c>
       <c r="B13" s="64">
-        <v>5939.4808502434344</v>
+        <v>5939.4808496909263</v>
       </c>
       <c r="C13" s="64">
-        <v>5355.6341088311647</v>
+        <v>5355.6341196997364</v>
       </c>
       <c r="D13" s="64">
-        <v>4729.5022790534067</v>
+        <v>4729.5022776459455</v>
       </c>
       <c r="E13" s="64">
-        <v>6248.9121016787512</v>
+        <v>6248.9120976163367</v>
       </c>
       <c r="F13" s="64">
-        <v>5038.9335234509126</v>
+        <v>5038.9335255713559</v>
       </c>
       <c r="G13" s="64">
-        <v>4650.8071985896086</v>
+        <v>4650.8072065351416</v>
       </c>
       <c r="H13" s="64">
-        <v>4914.5256520626535</v>
+        <v>4914.5256566934386</v>
       </c>
       <c r="I13" s="64">
         <v>-794.54064959259756</v>
@@ -16940,7 +16940,7 @@
         <v>-483.0663312724879</v>
       </c>
       <c r="N13" s="64">
-        <v>94.940012288013506</v>
+        <v>94.940012236274612</v>
       </c>
       <c r="O13" s="64">
         <v>97.176022350314497</v>
@@ -16994,7 +16994,7 @@
         <v>-9.0183508238887047</v>
       </c>
       <c r="AF13" s="64">
-        <v>94.940012288013506</v>
+        <v>94.940012236274612</v>
       </c>
       <c r="AG13" s="64">
         <v>45.894497192893652</v>
@@ -17034,25 +17034,25 @@
         <v>10</v>
       </c>
       <c r="B14" s="64">
-        <v>10999.365202043589</v>
+        <v>10999.365186860274</v>
       </c>
       <c r="C14" s="64">
-        <v>9601.1106770836814</v>
+        <v>9601.1106780987502</v>
       </c>
       <c r="D14" s="64">
-        <v>8416.8654965121659</v>
+        <v>8416.8655038119523</v>
       </c>
       <c r="E14" s="64">
-        <v>11264.053467258167</v>
+        <v>11264.053450204983</v>
       </c>
       <c r="F14" s="64">
-        <v>8681.5537560373614</v>
+        <v>8681.5537671566617</v>
       </c>
       <c r="G14" s="64">
-        <v>8056.8750986898067</v>
+        <v>8056.8751075874943</v>
       </c>
       <c r="H14" s="64">
-        <v>8331.2142455279609</v>
+        <v>8331.2142664894163</v>
       </c>
       <c r="I14" s="64">
         <v>-1609.6786169529412</v>
@@ -17070,7 +17070,7 @@
         <v>-718.73675307384087</v>
       </c>
       <c r="N14" s="64">
-        <v>94.058093635973151</v>
+        <v>94.058093504672925</v>
       </c>
       <c r="O14" s="64">
         <v>99.988964507246081</v>
@@ -17121,10 +17121,10 @@
         <v>-701.04347182540323</v>
       </c>
       <c r="AE14" s="64">
-        <v>-17.693281248437646</v>
+        <v>-17.693281248437643</v>
       </c>
       <c r="AF14" s="64">
-        <v>94.058093635973151</v>
+        <v>94.058093504672925</v>
       </c>
       <c r="AG14" s="64">
         <v>45.092389026061142</v>
@@ -17347,25 +17347,25 @@
         <v>1</v>
       </c>
       <c r="B17" s="64">
-        <v>785.8827932389388</v>
+        <v>785.88279228153647</v>
       </c>
       <c r="C17" s="64">
-        <v>1145.4956700163302</v>
+        <v>1145.4956702010536</v>
       </c>
       <c r="D17" s="64">
-        <v>742.57774004117573</v>
+        <v>742.57773916614758</v>
       </c>
       <c r="E17" s="64">
-        <v>1535.1743226048523</v>
+        <v>1535.1743196016453</v>
       </c>
       <c r="F17" s="64">
-        <v>1491.8692664036816</v>
+        <v>1491.8692664862563</v>
       </c>
       <c r="G17" s="64">
-        <v>1359.1014180813472</v>
+        <v>1359.101418236402</v>
       </c>
       <c r="H17" s="64">
-        <v>1442.7008084205113</v>
+        <v>1442.7008061606734</v>
       </c>
       <c r="I17" s="64">
         <v>-36.129532067293894</v>
@@ -17383,7 +17383,7 @@
         <v>-205.9201947554358</v>
       </c>
       <c r="N17" s="64">
-        <v>73.152346493314383</v>
+        <v>73.152346505581548</v>
       </c>
       <c r="O17" s="64">
         <v>40.74448150220622</v>
@@ -17434,10 +17434,10 @@
         <v>-204.18623741691835</v>
       </c>
       <c r="AE17" s="64">
-        <v>-1.7339573385174434</v>
+        <v>-1.7339573385174418</v>
       </c>
       <c r="AF17" s="64">
-        <v>73.152346493314383</v>
+        <v>73.152346505581548</v>
       </c>
       <c r="AG17" s="64">
         <v>3.2355782084791529</v>
@@ -17477,25 +17477,25 @@
         <v>2</v>
       </c>
       <c r="B18" s="64">
-        <v>1061.1589190688037</v>
+        <v>1061.1589180825042</v>
       </c>
       <c r="C18" s="64">
-        <v>1416.7366943978814</v>
+        <v>1416.736695130407</v>
       </c>
       <c r="D18" s="64">
-        <v>953.57361374687162</v>
+        <v>953.57361240082196</v>
       </c>
       <c r="E18" s="64">
-        <v>1791.170479909001</v>
+        <v>1791.1704803191756</v>
       </c>
       <c r="F18" s="64">
-        <v>1683.5851765888378</v>
+        <v>1683.5851746374931</v>
       </c>
       <c r="G18" s="64">
-        <v>1555.625205699168</v>
+        <v>1555.625202876229</v>
       </c>
       <c r="H18" s="64">
-        <v>1774.0265391660994</v>
+        <v>1774.0265434992759</v>
       </c>
       <c r="I18" s="64">
         <v>-84.577921811705139</v>
@@ -17513,7 +17513,7 @@
         <v>-206.75069480019278</v>
       </c>
       <c r="N18" s="64">
-        <v>78.790722921019437</v>
+        <v>78.790723038928633</v>
       </c>
       <c r="O18" s="64">
         <v>89.168210284756441</v>
@@ -17567,7 +17567,7 @@
         <v>-2.6272000895829715</v>
       </c>
       <c r="AF18" s="64">
-        <v>78.790722921019437</v>
+        <v>78.790723038928633</v>
       </c>
       <c r="AG18" s="64">
         <v>41.042856764702748</v>
@@ -17607,25 +17607,25 @@
         <v>3</v>
       </c>
       <c r="B19" s="64">
-        <v>1418.6743456117294</v>
+        <v>1418.6743428038731</v>
       </c>
       <c r="C19" s="64">
-        <v>1790.2405966042468</v>
+        <v>1790.2405975339038</v>
       </c>
       <c r="D19" s="64">
-        <v>1260.4932410798003</v>
+        <v>1260.493239579489</v>
       </c>
       <c r="E19" s="64">
-        <v>2126.9812684761773</v>
+        <v>2126.9812656037971</v>
       </c>
       <c r="F19" s="64">
-        <v>1968.8001629736671</v>
+        <v>1968.800162379413</v>
       </c>
       <c r="G19" s="64">
-        <v>1822.0079184833116</v>
+        <v>1822.0079205561058</v>
       </c>
       <c r="H19" s="64">
-        <v>2075.5596414704328</v>
+        <v>2075.5596468646359</v>
       </c>
       <c r="I19" s="64">
         <v>-119.15878297718137</v>
@@ -17643,7 +17643,7 @@
         <v>-228.52015254676397</v>
       </c>
       <c r="N19" s="64">
-        <v>81.727910751951001</v>
+        <v>81.727910723456802</v>
       </c>
       <c r="O19" s="64">
         <v>110.88489658522677</v>
@@ -17685,7 +17685,7 @@
         <v>127.72838769138772</v>
       </c>
       <c r="AB19" s="64">
-        <v>38.55433533045143</v>
+        <v>38.554335330451423</v>
       </c>
       <c r="AC19" s="64">
         <v>21.856548343567617</v>
@@ -17697,7 +17697,7 @@
         <v>-2.1553801294482131</v>
       </c>
       <c r="AF19" s="64">
-        <v>81.727910751951001</v>
+        <v>81.727910723456802</v>
       </c>
       <c r="AG19" s="64">
         <v>60.959213658984623</v>
@@ -17737,25 +17737,25 @@
         <v>4</v>
       </c>
       <c r="B20" s="64">
-        <v>1868.5291673894912</v>
+        <v>1868.5291655563055</v>
       </c>
       <c r="C20" s="64">
-        <v>2124.2456083889483</v>
+        <v>2124.2456078622286</v>
       </c>
       <c r="D20" s="64">
-        <v>1627.2560968178668</v>
+        <v>1627.2560952853516</v>
       </c>
       <c r="E20" s="64">
-        <v>2488.4560390199999</v>
+        <v>2488.4560352352182</v>
       </c>
       <c r="F20" s="64">
-        <v>2247.1829676341467</v>
+        <v>2247.1829649642641</v>
       </c>
       <c r="G20" s="64">
-        <v>2087.6852048045898</v>
+        <v>2087.6852054425831</v>
       </c>
       <c r="H20" s="64">
-        <v>2384.065402920301</v>
+        <v>2384.0653993961287</v>
       </c>
       <c r="I20" s="64">
         <v>-169.50713524076116</v>
@@ -17773,7 +17773,7 @@
         <v>-243.35577789208742</v>
       </c>
       <c r="N20" s="64">
-        <v>83.858018480827695</v>
+        <v>83.85801837040654</v>
       </c>
       <c r="O20" s="64">
         <v>145.25831873021318</v>
@@ -17824,10 +17824,10 @@
         <v>-240.04493054757413</v>
       </c>
       <c r="AE20" s="64">
-        <v>-3.3108473445133031</v>
+        <v>-3.3108473445133026</v>
       </c>
       <c r="AF20" s="64">
-        <v>83.858018480827695</v>
+        <v>83.85801837040654</v>
       </c>
       <c r="AG20" s="64">
         <v>97.718578539667291</v>
@@ -17867,25 +17867,25 @@
         <v>5</v>
       </c>
       <c r="B21" s="64">
-        <v>2353.8894973471606</v>
+        <v>2353.8895001209994</v>
       </c>
       <c r="C21" s="64">
-        <v>2548.0686270314864</v>
+        <v>2548.0686260020198</v>
       </c>
       <c r="D21" s="64">
-        <v>2020.560979288819</v>
+        <v>2020.5609773681233</v>
       </c>
       <c r="E21" s="64">
-        <v>2946.8419918047753</v>
+        <v>2946.8419915074892</v>
       </c>
       <c r="F21" s="64">
-        <v>2613.5134714692908</v>
+        <v>2613.5134687546133</v>
       </c>
       <c r="G21" s="64">
-        <v>2420.0745451103107</v>
+        <v>2420.0745444191157</v>
       </c>
       <c r="H21" s="64">
-        <v>2706.9091919885818</v>
+        <v>2706.9092010124687</v>
       </c>
       <c r="I21" s="64">
         <v>-240.75697755592472</v>
@@ -17903,7 +17903,7 @@
         <v>-282.20922624964362</v>
       </c>
       <c r="N21" s="64">
-        <v>88.770302008542927</v>
+        <v>88.770301914145861</v>
       </c>
       <c r="O21" s="64">
         <v>141.64167331180735</v>
@@ -17957,7 +17957,7 @@
         <v>-3.7461685801280034</v>
       </c>
       <c r="AF21" s="64">
-        <v>88.770302008542927</v>
+        <v>88.770301914145861</v>
       </c>
       <c r="AG21" s="64">
         <v>93.044234793460333</v>
@@ -17997,25 +17997,25 @@
         <v>6</v>
       </c>
       <c r="B22" s="64">
-        <v>2864.4380996295022</v>
+        <v>2864.4380995986967</v>
       </c>
       <c r="C22" s="64">
-        <v>2949.3073683871448</v>
+        <v>2949.3073668089537</v>
       </c>
       <c r="D22" s="64">
-        <v>2426.5007789486731</v>
+        <v>2426.5007793261489</v>
       </c>
       <c r="E22" s="64">
-        <v>3411.7501804694284</v>
+        <v>3411.7501786683506</v>
       </c>
       <c r="F22" s="64">
-        <v>2973.8128608880925</v>
+        <v>2973.8128583958028</v>
       </c>
       <c r="G22" s="64">
-        <v>2771.5449703256736</v>
+        <v>2771.544970422879</v>
       </c>
       <c r="H22" s="64">
-        <v>3115.3034912554485</v>
+        <v>3115.3034914885511</v>
       </c>
       <c r="I22" s="64">
         <v>-297.61816024008613</v>
@@ -18033,7 +18033,7 @@
         <v>-292.33435636543595</v>
       </c>
       <c r="N22" s="64">
-        <v>90.06646843950881</v>
+        <v>90.066468392512121</v>
       </c>
       <c r="O22" s="64">
         <v>161.69712739633152</v>
@@ -18084,10 +18084,10 @@
         <v>-287.51211729822063</v>
       </c>
       <c r="AE22" s="64">
-        <v>-4.8222390672153397</v>
+        <v>-4.8222390672153388</v>
       </c>
       <c r="AF22" s="64">
-        <v>90.06646843950881</v>
+        <v>90.066468392512121</v>
       </c>
       <c r="AG22" s="64">
         <v>111.96546757389082</v>
@@ -18127,25 +18127,25 @@
         <v>7</v>
       </c>
       <c r="B23" s="64">
-        <v>3573.3343063210036</v>
+        <v>3573.334296854558</v>
       </c>
       <c r="C23" s="64">
-        <v>3501.0868955659307</v>
+        <v>3501.0868922451186</v>
       </c>
       <c r="D23" s="64">
-        <v>2971.8896654777568</v>
+        <v>2971.8896625677053</v>
       </c>
       <c r="E23" s="64">
-        <v>4052.289566558381</v>
+        <v>4052.2895630832045</v>
       </c>
       <c r="F23" s="64">
-        <v>3450.844929506789</v>
+        <v>3450.8449287963513</v>
       </c>
       <c r="G23" s="64">
-        <v>3204.353770499943</v>
+        <v>3204.3537638873663</v>
       </c>
       <c r="H23" s="64">
-        <v>3540.1926659415717</v>
+        <v>3540.1926560797569</v>
       </c>
       <c r="I23" s="64">
         <v>-406.25656012065264</v>
@@ -18163,7 +18163,7 @@
         <v>-338.9402569978734</v>
       </c>
       <c r="N23" s="64">
-        <v>92.449092231782004</v>
+        <v>92.449092088888335</v>
       </c>
       <c r="O23" s="64">
         <v>160.86919232441272</v>
@@ -18214,10 +18214,10 @@
         <v>-333.4818149241753</v>
       </c>
       <c r="AE23" s="64">
-        <v>-5.4584420736981105</v>
+        <v>-5.4584420736981114</v>
       </c>
       <c r="AF23" s="64">
-        <v>92.449092231782004</v>
+        <v>92.449092088888335</v>
       </c>
       <c r="AG23" s="64">
         <v>112.13492564944744</v>
@@ -18257,25 +18257,25 @@
         <v>8</v>
       </c>
       <c r="B24" s="64">
-        <v>4462.5614045133761</v>
+        <v>4462.5613984095553</v>
       </c>
       <c r="C24" s="64">
-        <v>4269.6926527559453</v>
+        <v>4269.6926599898561</v>
       </c>
       <c r="D24" s="64">
-        <v>3641.6421684049747</v>
+        <v>3641.6421670842005</v>
       </c>
       <c r="E24" s="64">
-        <v>4955.3946264061215</v>
+        <v>4955.3946213516901</v>
       </c>
       <c r="F24" s="64">
-        <v>4134.4753925682744</v>
+        <v>4134.4753900263349</v>
       </c>
       <c r="G24" s="64">
-        <v>3826.5501767142027</v>
+        <v>3826.5501895663597</v>
       </c>
       <c r="H24" s="64">
-        <v>4139.9814588603585</v>
+        <v>4139.9814592594967</v>
       </c>
       <c r="I24" s="64">
         <v>-547.18664926276813</v>
@@ -18293,7 +18293,7 @@
         <v>-402.76742652978959</v>
       </c>
       <c r="N24" s="64">
-        <v>94.842226106416419</v>
+        <v>94.842226069813663</v>
       </c>
       <c r="O24" s="64">
         <v>151.48494499812023</v>
@@ -18341,13 +18341,13 @@
         <v>11.721667710936069</v>
       </c>
       <c r="AD24" s="64">
-        <v>-394.71928296201395</v>
+        <v>-394.71928296201389</v>
       </c>
       <c r="AE24" s="64">
         <v>-8.0481435677756306</v>
       </c>
       <c r="AF24" s="64">
-        <v>94.842226106416419</v>
+        <v>94.842226069813663</v>
       </c>
       <c r="AG24" s="64">
         <v>100.34264660010086</v>
@@ -18387,25 +18387,25 @@
         <v>9</v>
       </c>
       <c r="B25" s="64">
-        <v>5780.8996130640999</v>
+        <v>5780.8996216303522</v>
       </c>
       <c r="C25" s="64">
-        <v>5370.4217174053547</v>
+        <v>5370.4217173154002</v>
       </c>
       <c r="D25" s="64">
-        <v>4595.7718390208674</v>
+        <v>4595.7718360999415</v>
       </c>
       <c r="E25" s="64">
-        <v>6272.9289643102429</v>
+        <v>6272.9289675207147</v>
       </c>
       <c r="F25" s="64">
-        <v>5087.8011876150349</v>
+        <v>5087.8011819903031</v>
       </c>
       <c r="G25" s="64">
-        <v>4706.3329633294134</v>
+        <v>4706.3329717860752</v>
       </c>
       <c r="H25" s="64">
-        <v>5035.7196735747939</v>
+        <v>5035.7196799018675</v>
       </c>
       <c r="I25" s="64">
         <v>-774.28175819432408</v>
@@ -18423,7 +18423,7 @@
         <v>-477.09338586824231</v>
       </c>
       <c r="N25" s="64">
-        <v>95.625175798835301</v>
+        <v>95.625175664014662</v>
       </c>
       <c r="O25" s="64">
         <v>140.92430495854995</v>
@@ -18477,7 +18477,7 @@
         <v>-8.5999841050685522</v>
       </c>
       <c r="AF25" s="64">
-        <v>95.625175798835301</v>
+        <v>95.625175664014662</v>
       </c>
       <c r="AG25" s="64">
         <v>87.863888395875009</v>
@@ -18517,25 +18517,25 @@
         <v>10</v>
       </c>
       <c r="B26" s="64">
-        <v>10457.208548015204</v>
+        <v>10457.208530806187</v>
       </c>
       <c r="C26" s="64">
-        <v>9626.9512384307491</v>
+        <v>9626.9512465017706</v>
       </c>
       <c r="D26" s="64">
-        <v>8221.0964835156756</v>
+        <v>8221.096492059196</v>
       </c>
       <c r="E26" s="64">
-        <v>11144.281349469435</v>
+        <v>11144.281327044997</v>
       </c>
       <c r="F26" s="64">
-        <v>8908.1692719279199</v>
+        <v>8908.1692882980042</v>
       </c>
       <c r="G26" s="64">
-        <v>8318.9759451205828</v>
+        <v>8318.9759437204939</v>
       </c>
       <c r="H26" s="64">
-        <v>8670.2932244197782</v>
+        <v>8670.2932472507546</v>
       </c>
       <c r="I26" s="64">
         <v>-1386.1144909630011</v>
@@ -18553,7 +18553,7 @@
         <v>-682.26627280407808</v>
       </c>
       <c r="N26" s="64">
-        <v>93.072928347204254</v>
+        <v>93.072928226567015</v>
       </c>
       <c r="O26" s="64">
         <v>169.82684990837561</v>
@@ -18604,10 +18604,10 @@
         <v>-663.73247084133448</v>
       </c>
       <c r="AE26" s="64">
-        <v>-18.533801962743656</v>
+        <v>-18.533801962743652</v>
       </c>
       <c r="AF26" s="64">
-        <v>93.072928347204254</v>
+        <v>93.072928226567015</v>
       </c>
       <c r="AG26" s="64">
         <v>116.69260981539175</v>
@@ -18830,25 +18830,25 @@
         <v>156</v>
       </c>
       <c r="B29" s="64">
-        <v>6616.374903956651</v>
+        <v>6616.374892290698</v>
       </c>
       <c r="C29" s="64">
-        <v>5998.9860260517244</v>
+        <v>5998.9860366922376</v>
       </c>
       <c r="D29" s="64">
-        <v>5323.9161716662848</v>
+        <v>5323.9161641312558</v>
       </c>
       <c r="E29" s="64">
-        <v>7176.9202815275476</v>
+        <v>7176.920266089347</v>
       </c>
       <c r="F29" s="64">
-        <v>5884.4615418625517</v>
+        <v>5884.4615379299048</v>
       </c>
       <c r="G29" s="64">
-        <v>5435.472576094071</v>
+        <v>5435.4725659292371</v>
       </c>
       <c r="H29" s="64">
-        <v>5917.62269425048</v>
+        <v>5917.6226972864761</v>
       </c>
       <c r="I29" s="64">
         <v>-843.93158298412379</v>
@@ -18866,7 +18866,7 @@
         <v>-606.48761172308673</v>
       </c>
       <c r="N29" s="64">
-        <v>157.49863987663292</v>
+        <v>157.49863972241877</v>
       </c>
       <c r="O29" s="64">
         <v>187.20534317880262</v>
@@ -18908,7 +18908,7 @@
         <v>182.98631751387933</v>
       </c>
       <c r="AB29" s="64">
-        <v>63.989502648477774</v>
+        <v>63.989502648477767</v>
       </c>
       <c r="AC29" s="64">
         <v>13.973117183428128</v>
@@ -18920,7 +18920,7 @@
         <v>-10.359468007813129</v>
       </c>
       <c r="AF29" s="64">
-        <v>157.49863987663292</v>
+        <v>157.49863972241877</v>
       </c>
       <c r="AG29" s="64">
         <v>106.55264596375959</v>
@@ -18960,25 +18960,25 @@
         <v>157</v>
       </c>
       <c r="B30" s="64">
-        <v>5822.5747644569074</v>
+        <v>5822.5747553230258</v>
       </c>
       <c r="C30" s="64">
-        <v>5290.7919196305229</v>
+        <v>5290.7919201868817</v>
       </c>
       <c r="D30" s="64">
-        <v>4735.9488867858126</v>
+        <v>4735.9488892999561</v>
       </c>
       <c r="E30" s="64">
-        <v>6532.9256836569657</v>
+        <v>6532.92567134616</v>
       </c>
       <c r="F30" s="64">
-        <v>5446.2998054453828</v>
+        <v>5446.2998053230904</v>
       </c>
       <c r="G30" s="64">
-        <v>5082.9851000943008</v>
+        <v>5082.9851191385014</v>
       </c>
       <c r="H30" s="64">
-        <v>5688.6002882228613</v>
+        <v>5688.6002934191647</v>
       </c>
       <c r="I30" s="64">
         <v>-676.12230615307442</v>
@@ -18996,7 +18996,7 @@
         <v>-540.61897440868847</v>
       </c>
       <c r="N30" s="64">
-        <v>177.30428833018348</v>
+        <v>177.30428822409928</v>
       </c>
       <c r="O30" s="64">
         <v>158.4618644906167</v>
@@ -19050,7 +19050,7 @@
         <v>-9.7456285543548535</v>
       </c>
       <c r="AF30" s="64">
-        <v>177.30428833018348</v>
+        <v>177.30428822409928</v>
       </c>
       <c r="AG30" s="64">
         <v>67.563423381158742</v>
@@ -19090,25 +19090,25 @@
         <v>158</v>
       </c>
       <c r="B31" s="64">
-        <v>1875.09061170162</v>
+        <v>1875.0906106676866</v>
       </c>
       <c r="C31" s="64">
-        <v>1719.8582401796118</v>
+        <v>1719.8582442074289</v>
       </c>
       <c r="D31" s="64">
-        <v>1557.654110155923</v>
+        <v>1557.6541063616364</v>
       </c>
       <c r="E31" s="64">
-        <v>2339.9654405469018</v>
+        <v>2339.9654372874875</v>
       </c>
       <c r="F31" s="64">
-        <v>2022.5289393772946</v>
+        <v>2022.5289329814375</v>
       </c>
       <c r="G31" s="64">
-        <v>1912.1369969253149</v>
+        <v>1912.1370028561194</v>
       </c>
       <c r="H31" s="64">
-        <v>2282.7639494339364</v>
+        <v>2282.763948256134</v>
       </c>
       <c r="I31" s="64">
         <v>-203.18100661167026</v>
@@ -19126,7 +19126,7 @@
         <v>-196.18355600074409</v>
       </c>
       <c r="N31" s="64">
-        <v>85.791625889579564</v>
+        <v>85.791625875426107</v>
       </c>
       <c r="O31" s="64">
         <v>105.63315131788779</v>
@@ -19177,10 +19177,10 @@
         <v>-192.18251908849027</v>
       </c>
       <c r="AE31" s="64">
-        <v>-4.0010369122538103</v>
+        <v>-4.0010369122538094</v>
       </c>
       <c r="AF31" s="64">
-        <v>85.791625889579564</v>
+        <v>85.791625875426107</v>
       </c>
       <c r="AG31" s="64">
         <v>59.920200208036093</v>
@@ -19220,25 +19220,25 @@
         <v>159</v>
       </c>
       <c r="B32" s="64">
-        <v>1881.3798194842711</v>
+        <v>1881.3798185408357</v>
       </c>
       <c r="C32" s="64">
-        <v>1790.2791573250995</v>
+        <v>1790.2791594901207</v>
       </c>
       <c r="D32" s="64">
-        <v>1696.4263634729837</v>
+        <v>1696.4263630949822</v>
       </c>
       <c r="E32" s="64">
-        <v>2114.3975059948834</v>
+        <v>2114.3975034084278</v>
       </c>
       <c r="F32" s="64">
-        <v>1929.4440464540155</v>
+        <v>1929.4440479625739</v>
       </c>
       <c r="G32" s="64">
-        <v>1795.8327847592207</v>
+        <v>1795.832780968512</v>
       </c>
       <c r="H32" s="64">
-        <v>2066.8468826155326</v>
+        <v>2066.8468838879444</v>
       </c>
       <c r="I32" s="64">
         <v>-123.3153279715482</v>
@@ -19256,7 +19256,7 @@
         <v>-192.02013322874794</v>
       </c>
       <c r="N32" s="64">
-        <v>58.40886631402271</v>
+        <v>58.408866234685959</v>
       </c>
       <c r="O32" s="64">
         <v>62.803366650301477</v>
@@ -19307,10 +19307,10 @@
         <v>-188.02505041411555</v>
       </c>
       <c r="AE32" s="64">
-        <v>-3.9950828146323687</v>
+        <v>-3.9950828146323674</v>
       </c>
       <c r="AF32" s="64">
-        <v>58.40886631402271</v>
+        <v>58.408866234685959</v>
       </c>
       <c r="AG32" s="64">
         <v>28.939985557247372</v>
@@ -19350,25 +19350,25 @@
         <v>160</v>
       </c>
       <c r="B33" s="64">
-        <v>16080.808551952789</v>
+        <v>16080.808545516065</v>
       </c>
       <c r="C33" s="64">
-        <v>15241.167270295638</v>
+        <v>15241.167261615186</v>
       </c>
       <c r="D33" s="64">
-        <v>13082.334500062481</v>
+        <v>13082.334503898976</v>
       </c>
       <c r="E33" s="64">
-        <v>17543.946458435832</v>
+        <v>17543.946449944746</v>
       </c>
       <c r="F33" s="64">
-        <v>14545.472406412178</v>
+        <v>14545.472408327654</v>
       </c>
       <c r="G33" s="64">
-        <v>13483.908554966856</v>
+        <v>13483.908558265128</v>
       </c>
       <c r="H33" s="64">
-        <v>14182.228050416894</v>
+        <v>14182.228071090631</v>
       </c>
       <c r="I33" s="64">
         <v>-2012.7068984207851</v>
@@ -19386,7 +19386,7 @@
         <v>-1339.0438919151561</v>
       </c>
       <c r="N33" s="64">
-        <v>277.48004206882399</v>
+        <v>277.48004185263045</v>
       </c>
       <c r="O33" s="64">
         <v>420.46890102695943</v>
@@ -19440,7 +19440,7 @@
         <v>-24.82389791183553</v>
       </c>
       <c r="AF33" s="64">
-        <v>277.48004206882399</v>
+        <v>277.48004185263045</v>
       </c>
       <c r="AG33" s="64">
         <v>280.74314282257848</v>
@@ -19480,25 +19480,25 @@
         <v>161</v>
       </c>
       <c r="B34" s="64">
-        <v>1128.6194855309179</v>
+        <v>1128.6194850650288</v>
       </c>
       <c r="C34" s="64">
-        <v>3019.4571177199032</v>
+        <v>3019.4571189079379</v>
       </c>
       <c r="D34" s="64">
-        <v>1046.4993476431985</v>
+        <v>1046.499347561753</v>
       </c>
       <c r="E34" s="64">
-        <v>3137.0206630844159</v>
+        <v>3137.0206621143689</v>
       </c>
       <c r="F34" s="64">
-        <v>3054.9005246897923</v>
+        <v>3054.9005246110933</v>
       </c>
       <c r="G34" s="64">
-        <v>2801.1596169191862</v>
+        <v>2801.1596179243456</v>
       </c>
       <c r="H34" s="64">
-        <v>3070.537090653233</v>
+        <v>3070.5370930574827</v>
       </c>
       <c r="I34" s="64">
         <v>-60.841143423876936</v>
@@ -19516,7 +19516,7 @@
         <v>-324.01586491330653</v>
       </c>
       <c r="N34" s="64">
-        <v>70.274958200933028</v>
+        <v>70.274958226558937</v>
       </c>
       <c r="O34" s="64">
         <v>269.3774751331373</v>
@@ -19567,10 +19567,10 @@
         <v>-320.27112188978577</v>
       </c>
       <c r="AE34" s="64">
-        <v>-3.744743023520793</v>
+        <v>-3.7447430235207926</v>
       </c>
       <c r="AF34" s="64">
-        <v>70.274958200933028</v>
+        <v>70.274958226558937</v>
       </c>
       <c r="AG34" s="64">
         <v>202.05604600661971</v>
@@ -19610,25 +19610,25 @@
         <v>162</v>
       </c>
       <c r="B35" s="64">
-        <v>1221.7285571161535</v>
+        <v>1221.7285587412262</v>
       </c>
       <c r="C35" s="64">
-        <v>1681.707337781517</v>
+        <v>1681.7073384909181</v>
       </c>
       <c r="D35" s="64">
-        <v>1018.583226555798</v>
+        <v>1018.5832265885637</v>
       </c>
       <c r="E35" s="64">
-        <v>1880.0927557818648</v>
+        <v>1880.0927597457467</v>
       </c>
       <c r="F35" s="64">
-        <v>1676.9474233345204</v>
+        <v>1676.9474275930841</v>
       </c>
       <c r="G35" s="64">
-        <v>1560.7564884095941</v>
+        <v>1560.7564858317667</v>
       </c>
       <c r="H35" s="64">
-        <v>1676.1531424249395</v>
+        <v>1676.1531439157764</v>
       </c>
       <c r="I35" s="64">
         <v>-141.48970286861962</v>
@@ -19646,7 +19646,7 @@
         <v>-161.78771261981308</v>
       </c>
       <c r="N35" s="64">
-        <v>45.596770899226563</v>
+        <v>45.596770858495702</v>
       </c>
       <c r="O35" s="64">
         <v>108.54989820229473</v>
@@ -19700,7 +19700,7 @@
         <v>-2.3663070342807355</v>
       </c>
       <c r="AF35" s="64">
-        <v>45.596770899226563</v>
+        <v>45.596770858495702</v>
       </c>
       <c r="AG35" s="64">
         <v>79.224556060600008</v>
@@ -19923,25 +19923,25 @@
         <v>462</v>
       </c>
       <c r="B38" s="64">
-        <v>8154.8923408131086</v>
+        <v>8154.8923478919342</v>
       </c>
       <c r="C38" s="64">
-        <v>8523.1895021549353</v>
+        <v>8523.1895007088333</v>
       </c>
       <c r="D38" s="64">
-        <v>7040.9206486749054</v>
+        <v>7040.9206541559843</v>
       </c>
       <c r="E38" s="64">
-        <v>9828.7716785968205</v>
+        <v>9828.77168574188</v>
       </c>
       <c r="F38" s="64">
-        <v>8714.799987713046</v>
+        <v>8714.7999920059301</v>
       </c>
       <c r="G38" s="64">
-        <v>8160.9873249369548</v>
+        <v>8160.9873223449486</v>
       </c>
       <c r="H38" s="64">
-        <v>8967.78005743832</v>
+        <v>8967.7800666415988</v>
       </c>
       <c r="I38" s="64">
         <v>-757.07144782985563</v>
@@ -19959,7 +19959,7 @@
         <v>-799.67716690487418</v>
       </c>
       <c r="N38" s="64">
-        <v>245.86449745906538</v>
+        <v>245.864497243893</v>
       </c>
       <c r="O38" s="64">
         <v>411.37160568582084</v>
@@ -20013,7 +20013,7 @@
         <v>-11.103390059191726</v>
       </c>
       <c r="AF38" s="64">
-        <v>245.86449745906538</v>
+        <v>245.864497243893</v>
       </c>
       <c r="AG38" s="64">
         <v>281.19731847140309</v>
@@ -20053,25 +20053,25 @@
         <v>463</v>
       </c>
       <c r="B39" s="64">
-        <v>9220.2820098711618</v>
+        <v>9220.2819862262677</v>
       </c>
       <c r="C39" s="64">
-        <v>9412.5676400058728</v>
+        <v>9412.5676536450155</v>
       </c>
       <c r="D39" s="64">
-        <v>7758.4909356023063</v>
+        <v>7758.4909346986942</v>
       </c>
       <c r="E39" s="64">
-        <v>11017.728527583238</v>
+        <v>11017.728491487765</v>
       </c>
       <c r="F39" s="64">
-        <v>9555.9374379065066</v>
+        <v>9555.9374399601948</v>
       </c>
       <c r="G39" s="64">
-        <v>8851.79139629575</v>
+        <v>8851.7913809462189</v>
       </c>
       <c r="H39" s="64">
-        <v>9669.8019889763473</v>
+        <v>9669.8019883308571</v>
       </c>
       <c r="I39" s="64">
         <v>-990.54063218053261</v>
@@ -20089,7 +20089,7 @@
         <v>-958.13862316099539</v>
       </c>
       <c r="N39" s="64">
-        <v>253.99256428353763</v>
+        <v>253.99256414701932</v>
       </c>
       <c r="O39" s="64">
         <v>368.1173420477536</v>
@@ -20140,10 +20140,10 @@
         <v>-943.90023081128686</v>
       </c>
       <c r="AE39" s="64">
-        <v>-14.238392349708533</v>
+        <v>-14.238392349708528</v>
       </c>
       <c r="AF39" s="64">
-        <v>253.99256428353763</v>
+        <v>253.99256414701932</v>
       </c>
       <c r="AG39" s="64">
         <v>224.81626300331135</v>
@@ -20183,25 +20183,25 @@
         <v>464</v>
       </c>
       <c r="B40" s="64">
-        <v>4886.7085082212625</v>
+        <v>4886.708511057358</v>
       </c>
       <c r="C40" s="64">
-        <v>5197.9184757694256</v>
+        <v>5197.9184756886825</v>
       </c>
       <c r="D40" s="64">
-        <v>4172.760493202305</v>
+        <v>4172.7604902723215</v>
       </c>
       <c r="E40" s="64">
-        <v>6095.9358464544985</v>
+        <v>6095.935848798772</v>
       </c>
       <c r="F40" s="64">
-        <v>5381.9878326531598</v>
+        <v>5381.9878280137355</v>
       </c>
       <c r="G40" s="64">
-        <v>5044.0800681535038</v>
+        <v>5044.0800684175292</v>
       </c>
       <c r="H40" s="64">
-        <v>5551.8174875805889</v>
+        <v>5551.8174918120922</v>
       </c>
       <c r="I40" s="64">
         <v>-498.10486346291373</v>
@@ -20219,7 +20219,7 @@
         <v>-492.84148509649407</v>
       </c>
       <c r="N40" s="64">
-        <v>154.93372549699629</v>
+        <v>154.93372550028735</v>
       </c>
       <c r="O40" s="64">
         <v>260.68947589285619</v>
@@ -20261,7 +20261,7 @@
         <v>210.37473429582408</v>
       </c>
       <c r="AB40" s="64">
-        <v>98.979726705441863</v>
+        <v>98.979726705441877</v>
       </c>
       <c r="AC40" s="64">
         <v>31.290926633885078</v>
@@ -20273,7 +20273,7 @@
         <v>-4.9531516232953283</v>
       </c>
       <c r="AF40" s="64">
-        <v>154.93372549699629</v>
+        <v>154.93372550028735</v>
       </c>
       <c r="AG40" s="64">
         <v>168.82279989205722</v>
@@ -20313,25 +20313,25 @@
         <v>1238</v>
       </c>
       <c r="B41" s="64">
-        <v>12364.693835293776</v>
+        <v>12364.693820969009</v>
       </c>
       <c r="C41" s="64">
-        <v>11608.571451053784</v>
+        <v>11608.571449548177</v>
       </c>
       <c r="D41" s="64">
-        <v>9489.1905288629641</v>
+        <v>9489.1905218101256</v>
       </c>
       <c r="E41" s="64">
-        <v>13782.832736393853</v>
+        <v>13782.832723907863</v>
       </c>
       <c r="F41" s="64">
-        <v>10907.329429303023</v>
+        <v>10907.329424748978</v>
       </c>
       <c r="G41" s="64">
-        <v>10015.393328782335</v>
+        <v>10015.393359204914</v>
       </c>
       <c r="H41" s="64">
-        <v>10695.35256402262</v>
+        <v>10695.352584129065</v>
       </c>
       <c r="I41" s="64">
         <v>-1815.8710249603962</v>
@@ -20349,7 +20349,7 @@
         <v>-1109.5004696471794</v>
       </c>
       <c r="N41" s="64">
-        <v>217.56440433980296</v>
+        <v>217.56440410311552</v>
       </c>
       <c r="O41" s="64">
         <v>272.32157637356943</v>
@@ -20403,7 +20403,7 @@
         <v>-28.741230226495635</v>
       </c>
       <c r="AF41" s="64">
-        <v>217.56440433980296</v>
+        <v>217.56440410311552</v>
       </c>
       <c r="AG41" s="64">
         <v>150.1636186332284</v>
@@ -20626,25 +20626,25 @@
         <v>438</v>
       </c>
       <c r="B44" s="64">
-        <v>11868.474917246762</v>
+        <v>11868.474900756453</v>
       </c>
       <c r="C44" s="64">
-        <v>11206.124567013667</v>
+        <v>11206.124563995469</v>
       </c>
       <c r="D44" s="64">
-        <v>9128.9140840972614</v>
+        <v>9128.9140747464098</v>
       </c>
       <c r="E44" s="64">
-        <v>13276.10615078523</v>
+        <v>13276.106136699938</v>
       </c>
       <c r="F44" s="64">
-        <v>10536.545313134877</v>
+        <v>10536.545310689895</v>
       </c>
       <c r="G44" s="64">
-        <v>9659.2756021673449</v>
+        <v>9659.2756315665101</v>
       </c>
       <c r="H44" s="64">
-        <v>10329.930597429598</v>
+        <v>10329.930612363416</v>
       </c>
       <c r="I44" s="64">
         <v>-1722.9293893729823</v>
@@ -20662,7 +20662,7 @@
         <v>-1086.411174410046</v>
       </c>
       <c r="N44" s="64">
-        <v>209.14149544163971</v>
+        <v>209.14149528665965</v>
       </c>
       <c r="O44" s="64">
         <v>259.40640073403409</v>
@@ -20716,7 +20716,7 @@
         <v>-29.060021896711756</v>
       </c>
       <c r="AF44" s="64">
-        <v>209.14149544163971</v>
+        <v>209.14149528665965</v>
       </c>
       <c r="AG44" s="64">
         <v>141.5644712296654</v>
@@ -20756,25 +20756,25 @@
         <v>439</v>
       </c>
       <c r="B45" s="64">
-        <v>5473.2385594597517</v>
+        <v>5473.2385585318525</v>
       </c>
       <c r="C45" s="64">
-        <v>5556.0128538011886</v>
+        <v>5556.012855009094</v>
       </c>
       <c r="D45" s="64">
-        <v>4423.3089675309984</v>
+        <v>4423.3089600861776</v>
       </c>
       <c r="E45" s="64">
-        <v>6548.7767733269675</v>
+        <v>6548.7767686227407</v>
       </c>
       <c r="F45" s="64">
-        <v>5498.8471805419131</v>
+        <v>5498.8471701770659</v>
       </c>
       <c r="G45" s="64">
-        <v>5071.618906202968</v>
+        <v>5071.6189012243267</v>
       </c>
       <c r="H45" s="64">
-        <v>5602.4905549651412</v>
+        <v>5602.4905712343325</v>
       </c>
       <c r="I45" s="64">
         <v>-707.90045122783397</v>
@@ -20792,7 +20792,7 @@
         <v>-579.24914274689877</v>
       </c>
       <c r="N45" s="64">
-        <v>152.02087404324195</v>
+        <v>152.02087379416031</v>
       </c>
       <c r="O45" s="64">
         <v>234.20935967434758</v>
@@ -20843,10 +20843,10 @@
         <v>-571.63399909453653</v>
       </c>
       <c r="AE45" s="64">
-        <v>-7.6151436523622777</v>
+        <v>-7.6151436523622769</v>
       </c>
       <c r="AF45" s="64">
-        <v>152.02087404324195</v>
+        <v>152.02087379416031</v>
       </c>
       <c r="AG45" s="64">
         <v>148.10644259542411</v>
@@ -20886,25 +20886,25 @@
         <v>440</v>
       </c>
       <c r="B46" s="64">
-        <v>17284.863217492799</v>
+        <v>17284.863206856262</v>
       </c>
       <c r="C46" s="64">
-        <v>17980.109648169164</v>
+        <v>17980.109660586149</v>
       </c>
       <c r="D46" s="64">
-        <v>14909.139554714222</v>
+        <v>14909.139566104535</v>
       </c>
       <c r="E46" s="64">
-        <v>20900.385864916214</v>
+        <v>20900.3858446136</v>
       </c>
       <c r="F46" s="64">
-        <v>18524.662193898945</v>
+        <v>18524.662203861877</v>
       </c>
       <c r="G46" s="64">
-        <v>17341.357609798233</v>
+        <v>17341.357598122773</v>
       </c>
       <c r="H46" s="64">
-        <v>18952.33094562314</v>
+        <v>18952.330947315862</v>
       </c>
       <c r="I46" s="64">
         <v>-1630.7581278328821</v>
@@ -20922,7 +20922,7 @@
         <v>-1694.4974276525979</v>
       </c>
       <c r="N46" s="64">
-        <v>511.19282209452064</v>
+        <v>511.19282191349521</v>
       </c>
       <c r="O46" s="64">
         <v>818.88423959161832</v>
@@ -20973,10 +20973,10 @@
         <v>-1672.1364289429807</v>
       </c>
       <c r="AE46" s="64">
-        <v>-22.360998709617185</v>
+        <v>-22.360998709617181</v>
       </c>
       <c r="AF46" s="64">
-        <v>511.19282209452064</v>
+        <v>511.19282191349521</v>
       </c>
       <c r="AG46" s="64">
         <v>535.32908617491057</v>
@@ -21277,7 +21277,7 @@
         <v>1000000</v>
       </c>
       <c r="E5" s="13">
-        <v>0.17716056995546786</v>
+        <v>0.17716056985615253</v>
       </c>
       <c r="F5" t="s">
         <v>163</v>
@@ -21321,7 +21321,7 @@
         <v>1000000</v>
       </c>
       <c r="E6" s="13">
-        <v>0.12407229694866895</v>
+        <v>0.12407229702605803</v>
       </c>
       <c r="F6" t="s">
         <v>163</v>
@@ -21497,7 +21497,7 @@
         <v>1000000</v>
       </c>
       <c r="E10" s="13">
-        <v>0.077555408065401066</v>
+        <v>0.077555407906039403</v>
       </c>
       <c r="F10" t="s">
         <v>164</v>
@@ -21541,7 +21541,7 @@
         <v>1000000</v>
       </c>
       <c r="E11" s="13">
-        <v>0.038805543569967751</v>
+        <v>0.038805543561015322</v>
       </c>
       <c r="F11" t="s">
         <v>164</v>
@@ -21717,7 +21717,7 @@
         <v>1000000</v>
       </c>
       <c r="E15" s="13">
-        <v>0.19011822173618598</v>
+        <v>0.19011822164280867</v>
       </c>
       <c r="F15" t="s">
         <v>165</v>
@@ -21761,7 +21761,7 @@
         <v>1000000</v>
       </c>
       <c r="E16" s="13">
-        <v>0.12926614806340578</v>
+        <v>0.12926614813252724</v>
       </c>
       <c r="F16" t="s">
         <v>165</v>
@@ -21937,7 +21937,7 @@
         <v>1000000</v>
       </c>
       <c r="E20" s="13">
-        <v>0.026361890364144627</v>
+        <v>0.026361890258195336</v>
       </c>
       <c r="F20" t="s">
         <v>166</v>
@@ -21981,7 +21981,7 @@
         <v>1000000</v>
       </c>
       <c r="E21" s="13">
-        <v>0.0046525425146296115</v>
+        <v>0.0046525425759336228</v>
       </c>
       <c r="F21" t="s">
         <v>166</v>
@@ -22157,7 +22157,7 @@
         <v>1000000</v>
       </c>
       <c r="E25" s="13">
-        <v>0.031466143766107547</v>
+        <v>0.031466143453894931</v>
       </c>
       <c r="F25" t="s">
         <v>167</v>
@@ -22201,7 +22201,7 @@
         <v>1000000</v>
       </c>
       <c r="E26" s="13">
-        <v>0.0056948804505994903</v>
+        <v>0.0056948805543970051</v>
       </c>
       <c r="F26" t="s">
         <v>167</v>
@@ -22377,7 +22377,7 @@
         <v>1000000</v>
       </c>
       <c r="E30" s="13">
-        <v>0.046182869171644117</v>
+        <v>0.046182869466039979</v>
       </c>
       <c r="F30" t="s">
         <v>168</v>
@@ -22421,7 +22421,7 @@
         <v>1000000</v>
       </c>
       <c r="E31" s="13">
-        <v>0.010590045984474203</v>
+        <v>0.010590046013096519</v>
       </c>
       <c r="F31" t="s">
         <v>168</v>
@@ -22597,7 +22597,7 @@
         <v>1000000</v>
       </c>
       <c r="E35" s="13">
-        <v>0.022553174967749914</v>
+        <v>0.022553174940164917</v>
       </c>
       <c r="F35" t="s">
         <v>169</v>
@@ -22641,7 +22641,7 @@
         <v>1000000</v>
       </c>
       <c r="E36" s="13">
-        <v>0.0045255200307917692</v>
+        <v>0.0045255200862868612</v>
       </c>
       <c r="F36" t="s">
         <v>169</v>
@@ -24265,67 +24265,67 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>222.64691523122787</v>
+        <v>222.64691519176475</v>
       </c>
       <c r="B3">
-        <v>39.337630168914792</v>
+        <v>39.33763023481945</v>
       </c>
       <c r="C3">
-        <v>1.0010235729217529</v>
+        <v>1.0010235857208631</v>
       </c>
       <c r="D3">
-        <v>273.8001742606163</v>
+        <v>273.8001742207814</v>
       </c>
       <c r="E3">
-        <v>281.99211425065994</v>
+        <v>281.99211408367324</v>
       </c>
       <c r="F3">
-        <v>200.35290495967865</v>
+        <v>200.35290494846654</v>
       </c>
       <c r="G3">
-        <v>216.30692843246459</v>
+        <v>216.30692849346809</v>
       </c>
       <c r="H3">
-        <v>191.42274833488463</v>
+        <v>191.42274824547948</v>
       </c>
       <c r="I3">
-        <v>21.789254470825195</v>
+        <v>21.789254561996167</v>
       </c>
       <c r="J3">
-        <v>1.941918454170227</v>
+        <v>1.9419184629179833</v>
       </c>
       <c r="K3">
-        <v>127.06205954933166</v>
+        <v>127.06205957215185</v>
       </c>
       <c r="L3">
-        <v>42.98450095129013</v>
+        <v>42.984500919368109</v>
       </c>
       <c r="M3">
-        <v>44.946022023200989</v>
+        <v>44.946022082656803</v>
       </c>
       <c r="N3">
-        <v>424.87732813739774</v>
+        <v>424.87732793347396</v>
       </c>
       <c r="O3">
-        <v>341.42592822885513</v>
+        <v>341.20272449479899</v>
       </c>
       <c r="P3">
-        <v>423.74766212558745</v>
+        <v>423.74766191820925</v>
       </c>
       <c r="Q3">
-        <v>69.322490505695342</v>
+        <v>69.322490518232144</v>
       </c>
       <c r="R3">
-        <v>384.11934976005557</v>
+        <v>384.11934960941642</v>
       </c>
       <c r="S3">
-        <v>46.406511035919188</v>
+        <v>46.406511068090026</v>
       </c>
       <c r="T3">
-        <v>94.257799573898311</v>
+        <v>94.257799554629528</v>
       </c>
       <c r="U3">
-        <v>16.978020687103271</v>
+        <v>16.978020724909324</v>
       </c>
     </row>
     <row r="5">
@@ -24442,7 +24442,7 @@
         <v>1000</v>
       </c>
       <c r="O7">
-        <v>842.41474038752642</v>
+        <v>841.81839252430132</v>
       </c>
       <c r="P7">
         <v>998.02895854424685</v>
@@ -26367,7 +26367,7 @@
         <v>378</v>
       </c>
       <c r="D9" s="13">
-        <v>711.87945053617239</v>
+        <v>711.8794516149311</v>
       </c>
       <c r="E9" s="13">
         <v>99983.870481725811</v>
@@ -26607,7 +26607,7 @@
         <v>378</v>
       </c>
       <c r="D21" s="13">
-        <v>711.87945053617239</v>
+        <v>711.8794516149311</v>
       </c>
       <c r="E21" s="13">
         <v>99983.870481725811</v>
@@ -26687,7 +26687,7 @@
         <v>378</v>
       </c>
       <c r="D25" s="13">
-        <v>2022.6332824077292</v>
+        <v>2022.6332827493518</v>
       </c>
       <c r="E25" s="13">
         <v>99983.870481725811</v>
@@ -26707,7 +26707,7 @@
         <v>378</v>
       </c>
       <c r="D26" s="13">
-        <v>16226.826396851777</v>
+        <v>16226.82640272</v>
       </c>
       <c r="E26" s="13">
         <v>99983.870481725811</v>
@@ -26727,7 +26727,7 @@
         <v>378</v>
       </c>
       <c r="D27" s="13">
-        <v>2012.9242863257589</v>
+        <v>2012.9242863570623</v>
       </c>
       <c r="E27" s="13">
         <v>99983.870481725811</v>
@@ -26747,7 +26747,7 @@
         <v>378</v>
       </c>
       <c r="D28" s="13">
-        <v>19274.483948472076</v>
+        <v>19274.483951255002</v>
       </c>
       <c r="E28" s="13">
         <v>99983.870481725811</v>
@@ -26767,7 +26767,7 @@
         <v>378</v>
       </c>
       <c r="D29" s="13">
-        <v>19264.774956196812</v>
+        <v>19264.774954862714</v>
       </c>
       <c r="E29" s="13">
         <v>99983.870481725811</v>
@@ -26787,7 +26787,7 @@
         <v>378</v>
       </c>
       <c r="D30" s="13">
-        <v>17534.641919991409</v>
+        <v>17534.641906996003</v>
       </c>
       <c r="E30" s="13">
         <v>99983.870481725811</v>
@@ -26807,7 +26807,7 @@
         <v>378</v>
       </c>
       <c r="D31" s="13">
-        <v>20466.326067515129</v>
+        <v>20466.326047533457</v>
       </c>
       <c r="E31" s="13">
         <v>99983.870481725811</v>
@@ -27007,7 +27007,7 @@
         <v>378</v>
       </c>
       <c r="D41" s="13">
-        <v>2020.4226071964447</v>
+        <v>2020.4226071964449</v>
       </c>
       <c r="E41" s="13">
         <v>99988.831005234359</v>
@@ -27087,7 +27087,7 @@
         <v>378</v>
       </c>
       <c r="D45" s="13">
-        <v>754.66031951255104</v>
+        <v>754.66031922954585</v>
       </c>
       <c r="E45" s="13">
         <v>99988.831005234359</v>
@@ -27327,7 +27327,7 @@
         <v>378</v>
       </c>
       <c r="D57" s="13">
-        <v>754.66031951255104</v>
+        <v>754.66031922954585</v>
       </c>
       <c r="E57" s="13">
         <v>99988.831005234359</v>
@@ -27407,7 +27407,7 @@
         <v>378</v>
       </c>
       <c r="D61" s="13">
-        <v>7238.0377497152194</v>
+        <v>7238.0377417416039</v>
       </c>
       <c r="E61" s="13">
         <v>99988.831005234359</v>
@@ -27427,7 +27427,7 @@
         <v>378</v>
       </c>
       <c r="D62" s="13">
-        <v>14297.479642375662</v>
+        <v>14297.479635078827</v>
       </c>
       <c r="E62" s="13">
         <v>99988.831005234359</v>
@@ -27447,7 +27447,7 @@
         <v>378</v>
       </c>
       <c r="D63" s="13">
-        <v>7085.9449377849114</v>
+        <v>7085.9449342793123</v>
       </c>
       <c r="E63" s="13">
         <v>99988.831005234359</v>
@@ -27467,7 +27467,7 @@
         <v>378</v>
       </c>
       <c r="D64" s="13">
-        <v>18086.056022547087</v>
+        <v>18086.056041135824</v>
       </c>
       <c r="E64" s="13">
         <v>99988.831005234359</v>
@@ -27487,7 +27487,7 @@
         <v>378</v>
       </c>
       <c r="D65" s="13">
-        <v>17933.963230651345</v>
+        <v>17933.963233673534</v>
       </c>
       <c r="E65" s="13">
         <v>99988.831005234359</v>
@@ -27507,7 +27507,7 @@
         <v>378</v>
       </c>
       <c r="D66" s="13">
-        <v>16679.290389569767</v>
+        <v>16679.290404946882</v>
       </c>
       <c r="E66" s="13">
         <v>99988.831005234359</v>
@@ -27527,7 +27527,7 @@
         <v>378</v>
       </c>
       <c r="D67" s="13">
-        <v>19603.080082470835</v>
+        <v>19603.080083207955</v>
       </c>
       <c r="E67" s="13">
         <v>99988.831005234359</v>
@@ -27727,7 +27727,7 @@
         <v>378</v>
       </c>
       <c r="D77" s="13">
-        <v>437.72893591580146</v>
+        <v>437.72893591580134</v>
       </c>
       <c r="E77" s="13">
         <v>99998.609302509212</v>
@@ -27787,7 +27787,7 @@
         <v>378</v>
       </c>
       <c r="D80" s="13">
-        <v>24.009123198230782</v>
+        <v>24.009123198230771</v>
       </c>
       <c r="E80" s="13">
         <v>99998.609302509212</v>
@@ -27807,7 +27807,7 @@
         <v>378</v>
       </c>
       <c r="D81" s="13">
-        <v>853.21177831026716</v>
+        <v>853.21177907939045</v>
       </c>
       <c r="E81" s="13">
         <v>99998.609302509212</v>
@@ -28047,7 +28047,7 @@
         <v>378</v>
       </c>
       <c r="D93" s="13">
-        <v>853.21177831026716</v>
+        <v>853.21177907939045</v>
       </c>
       <c r="E93" s="13">
         <v>99998.609302509212</v>
@@ -28127,7 +28127,7 @@
         <v>378</v>
       </c>
       <c r="D97" s="13">
-        <v>13170.968621871985</v>
+        <v>13170.968626034593</v>
       </c>
       <c r="E97" s="13">
         <v>99998.609302509212</v>
@@ -28147,7 +28147,7 @@
         <v>378</v>
       </c>
       <c r="D98" s="13">
-        <v>16432.956358121261</v>
+        <v>16432.956354300899</v>
       </c>
       <c r="E98" s="13">
         <v>99998.609302509212</v>
@@ -28167,7 +28167,7 @@
         <v>378</v>
       </c>
       <c r="D99" s="13">
-        <v>12417.36105775828</v>
+        <v>12417.361060163843</v>
       </c>
       <c r="E99" s="13">
         <v>99998.609302509212</v>
@@ -28187,7 +28187,7 @@
         <v>378</v>
       </c>
       <c r="D100" s="13">
-        <v>19581.846409622904</v>
+        <v>19581.84638577644</v>
       </c>
       <c r="E100" s="13">
         <v>99998.609302509212</v>
@@ -28207,7 +28207,7 @@
         <v>378</v>
       </c>
       <c r="D101" s="13">
-        <v>18828.238824045457</v>
+        <v>18828.238819905688</v>
       </c>
       <c r="E101" s="13">
         <v>99998.609302509212</v>
@@ -28227,7 +28227,7 @@
         <v>378</v>
       </c>
       <c r="D102" s="13">
-        <v>17604.248582438504</v>
+        <v>17604.248548433654</v>
       </c>
       <c r="E102" s="13">
         <v>99998.609302509212</v>
@@ -28247,7 +28247,7 @@
         <v>378</v>
       </c>
       <c r="D103" s="13">
-        <v>20164.140389506341</v>
+        <v>20164.140422756969</v>
       </c>
       <c r="E103" s="13">
         <v>99998.609302509212</v>
@@ -28507,7 +28507,7 @@
         <v>378</v>
       </c>
       <c r="D116" s="13">
-        <v>29.888966764581458</v>
+        <v>29.888966764581451</v>
       </c>
       <c r="E116" s="13">
         <v>99992.252291726545</v>
@@ -28527,7 +28527,7 @@
         <v>378</v>
       </c>
       <c r="D117" s="13">
-        <v>854.92595549449504</v>
+        <v>854.92595474789539</v>
       </c>
       <c r="E117" s="13">
         <v>99992.252291726545</v>
@@ -28767,7 +28767,7 @@
         <v>378</v>
       </c>
       <c r="D129" s="13">
-        <v>854.92595549449504</v>
+        <v>854.92595474789539</v>
       </c>
       <c r="E129" s="13">
         <v>99992.252291726545</v>
@@ -28847,7 +28847,7 @@
         <v>378</v>
       </c>
       <c r="D133" s="13">
-        <v>18566.158867702783</v>
+        <v>18566.158809941753</v>
       </c>
       <c r="E133" s="13">
         <v>99992.252291726545</v>
@@ -28867,7 +28867,7 @@
         <v>378</v>
       </c>
       <c r="D134" s="13">
-        <v>20161.24183383954</v>
+        <v>20161.241818124741</v>
       </c>
       <c r="E134" s="13">
         <v>99992.252291726545</v>
@@ -28887,7 +28887,7 @@
         <v>378</v>
       </c>
       <c r="D135" s="13">
-        <v>16786.83980848841</v>
+        <v>16786.83980828623</v>
       </c>
       <c r="E135" s="13">
         <v>99992.252291726545</v>
@@ -28907,7 +28907,7 @@
         <v>378</v>
       </c>
       <c r="D136" s="13">
-        <v>23587.434570471043</v>
+        <v>23587.434516346806</v>
       </c>
       <c r="E136" s="13">
         <v>99992.252291726545</v>
@@ -28927,7 +28927,7 @@
         <v>378</v>
       </c>
       <c r="D137" s="13">
-        <v>21808.115537425088</v>
+        <v>21808.115514691286</v>
       </c>
       <c r="E137" s="13">
         <v>99992.252291726545</v>
@@ -28947,7 +28947,7 @@
         <v>378</v>
       </c>
       <c r="D138" s="13">
-        <v>20433.547597900138</v>
+        <v>20433.547640440403</v>
       </c>
       <c r="E138" s="13">
         <v>99992.252291726545</v>
@@ -28967,7 +28967,7 @@
         <v>378</v>
       </c>
       <c r="D139" s="13">
-        <v>23702.007356239184</v>
+        <v>23702.007404602689</v>
       </c>
       <c r="E139" s="13">
         <v>99992.252291726545</v>
@@ -29227,7 +29227,7 @@
         <v>378</v>
       </c>
       <c r="D152" s="13">
-        <v>41.749080466323967</v>
+        <v>41.74908046632396</v>
       </c>
       <c r="E152" s="13">
         <v>99939.229778800975</v>
@@ -29247,7 +29247,7 @@
         <v>378</v>
       </c>
       <c r="D153" s="13">
-        <v>870.19205761132116</v>
+        <v>870.19205699208874</v>
       </c>
       <c r="E153" s="13">
         <v>99939.229778800975</v>
@@ -29487,7 +29487,7 @@
         <v>378</v>
       </c>
       <c r="D165" s="13">
-        <v>870.19205761132116</v>
+        <v>870.19205699208874</v>
       </c>
       <c r="E165" s="13">
         <v>99939.229778800975</v>
@@ -29567,7 +29567,7 @@
         <v>378</v>
       </c>
       <c r="D169" s="13">
-        <v>23576.374253835431</v>
+        <v>23576.37430423461</v>
       </c>
       <c r="E169" s="13">
         <v>99939.229778800975</v>
@@ -29587,7 +29587,7 @@
         <v>378</v>
       </c>
       <c r="D170" s="13">
-        <v>24348.023207157232</v>
+        <v>24348.023221690666</v>
       </c>
       <c r="E170" s="13">
         <v>99939.229778800975</v>
@@ -29607,7 +29607,7 @@
         <v>378</v>
       </c>
       <c r="D171" s="13">
-        <v>20927.531991160769</v>
+        <v>20927.531966903265</v>
       </c>
       <c r="E171" s="13">
         <v>99939.229778800975</v>
@@ -29627,7 +29627,7 @@
         <v>378</v>
       </c>
       <c r="D172" s="13">
-        <v>28444.990900674282</v>
+        <v>28444.990892798633</v>
       </c>
       <c r="E172" s="13">
         <v>99939.229778800975</v>
@@ -29647,7 +29647,7 @@
         <v>378</v>
       </c>
       <c r="D173" s="13">
-        <v>25796.1485679133</v>
+        <v>25796.148555467287</v>
       </c>
       <c r="E173" s="13">
         <v>99939.229778800975</v>
@@ -29667,7 +29667,7 @@
         <v>378</v>
       </c>
       <c r="D174" s="13">
-        <v>23940.210539790103</v>
+        <v>23940.210541473007</v>
       </c>
       <c r="E174" s="13">
         <v>99939.229778800975</v>
@@ -29687,7 +29687,7 @@
         <v>378</v>
       </c>
       <c r="D175" s="13">
-        <v>26689.813460680209</v>
+        <v>26689.813459963763</v>
       </c>
       <c r="E175" s="13">
         <v>99939.229778800975</v>
@@ -29927,7 +29927,7 @@
         <v>378</v>
       </c>
       <c r="D187" s="13">
-        <v>2870.9901455614163</v>
+        <v>2870.9901455614158</v>
       </c>
       <c r="E187" s="13">
         <v>99981.531562891876</v>
@@ -29967,7 +29967,7 @@
         <v>378</v>
       </c>
       <c r="D189" s="13">
-        <v>919.26665957818068</v>
+        <v>919.26665888861214</v>
       </c>
       <c r="E189" s="13">
         <v>99981.531562891876</v>
@@ -30207,7 +30207,7 @@
         <v>378</v>
       </c>
       <c r="D201" s="13">
-        <v>919.26665957818068</v>
+        <v>919.26665888861214</v>
       </c>
       <c r="E201" s="13">
         <v>99981.531562891876</v>
@@ -30287,7 +30287,7 @@
         <v>378</v>
       </c>
       <c r="D205" s="13">
-        <v>29812.112471137836</v>
+        <v>29812.112476153972</v>
       </c>
       <c r="E205" s="13">
         <v>99981.531562891876</v>
@@ -30307,7 +30307,7 @@
         <v>378</v>
       </c>
       <c r="D206" s="13">
-        <v>29607.570849675511</v>
+        <v>29607.570839122476</v>
       </c>
       <c r="E206" s="13">
         <v>99981.531562891876</v>
@@ -30327,7 +30327,7 @@
         <v>378</v>
       </c>
       <c r="D207" s="13">
-        <v>25900.464251206122</v>
+        <v>25900.464240839785</v>
       </c>
       <c r="E207" s="13">
         <v>99981.531562891876</v>
@@ -30347,7 +30347,7 @@
         <v>378</v>
       </c>
       <c r="D208" s="13">
-        <v>33851.270984779578</v>
+        <v>33851.271009985874</v>
       </c>
       <c r="E208" s="13">
         <v>99981.531562891876</v>
@@ -30367,7 +30367,7 @@
         <v>378</v>
       </c>
       <c r="D209" s="13">
-        <v>29939.622783442624</v>
+        <v>29939.622774671676</v>
       </c>
       <c r="E209" s="13">
         <v>99981.531562891876</v>
@@ -30387,7 +30387,7 @@
         <v>378</v>
       </c>
       <c r="D210" s="13">
-        <v>27939.22089348374</v>
+        <v>27939.220833174481</v>
       </c>
       <c r="E210" s="13">
         <v>99981.531562891876</v>
@@ -30407,7 +30407,7 @@
         <v>378</v>
       </c>
       <c r="D211" s="13">
-        <v>30719.43650397057</v>
+        <v>30719.436474669572</v>
       </c>
       <c r="E211" s="13">
         <v>99981.531562891876</v>
@@ -30687,7 +30687,7 @@
         <v>378</v>
       </c>
       <c r="D225" s="13">
-        <v>920.64636027014433</v>
+        <v>920.64635780566687</v>
       </c>
       <c r="E225" s="13">
         <v>100083.43794638522</v>
@@ -30927,7 +30927,7 @@
         <v>378</v>
       </c>
       <c r="D237" s="13">
-        <v>920.64636027014433</v>
+        <v>920.64635780566687</v>
       </c>
       <c r="E237" s="13">
         <v>100083.43794638522</v>
@@ -31007,7 +31007,7 @@
         <v>378</v>
       </c>
       <c r="D241" s="13">
-        <v>36619.893713286612</v>
+        <v>36619.893670342324</v>
       </c>
       <c r="E241" s="13">
         <v>100083.43794638522</v>
@@ -31027,7 +31027,7 @@
         <v>378</v>
       </c>
       <c r="D242" s="13">
-        <v>33882.873102853657</v>
+        <v>33882.873082739359</v>
       </c>
       <c r="E242" s="13">
         <v>100083.43794638522</v>
@@ -31047,7 +31047,7 @@
         <v>378</v>
       </c>
       <c r="D243" s="13">
-        <v>30293.219645284054</v>
+        <v>30293.219588319491</v>
       </c>
       <c r="E243" s="13">
         <v>100083.43794638522</v>
@@ -31067,7 +31067,7 @@
         <v>378</v>
       </c>
       <c r="D244" s="13">
-        <v>39798.42211136355</v>
+        <v>39798.422051391804</v>
       </c>
       <c r="E244" s="13">
         <v>100083.43794638522</v>
@@ -31087,7 +31087,7 @@
         <v>378</v>
       </c>
       <c r="D245" s="13">
-        <v>33471.74803862314</v>
+        <v>33471.747969368967</v>
       </c>
       <c r="E245" s="13">
         <v>100083.43794638522</v>
@@ -31107,7 +31107,7 @@
         <v>378</v>
       </c>
       <c r="D246" s="13">
-        <v>31071.603212597944</v>
+        <v>31071.603272909135</v>
       </c>
       <c r="E246" s="13">
         <v>100083.43794638522</v>
@@ -31127,7 +31127,7 @@
         <v>378</v>
       </c>
       <c r="D247" s="13">
-        <v>33955.569591860833</v>
+        <v>33955.569594606997</v>
       </c>
       <c r="E247" s="13">
         <v>100083.43794638522</v>
@@ -31407,7 +31407,7 @@
         <v>378</v>
       </c>
       <c r="D261" s="13">
-        <v>949.4914411741936</v>
+        <v>949.49144010980774</v>
       </c>
       <c r="E261" s="13">
         <v>99947.811107758622</v>
@@ -31647,7 +31647,7 @@
         <v>378</v>
       </c>
       <c r="D273" s="13">
-        <v>949.4914411741936</v>
+        <v>949.49144010980774</v>
       </c>
       <c r="E273" s="13">
         <v>99947.811107758622</v>
@@ -31727,7 +31727,7 @@
         <v>378</v>
       </c>
       <c r="D277" s="13">
-        <v>45887.110069555536</v>
+        <v>45887.109995149032</v>
       </c>
       <c r="E277" s="13">
         <v>99947.811107758622</v>
@@ -31747,7 +31747,7 @@
         <v>378</v>
       </c>
       <c r="D278" s="13">
-        <v>42918.448092707935</v>
+        <v>42918.448117071355</v>
       </c>
       <c r="E278" s="13">
         <v>99947.811107758622</v>
@@ -31767,7 +31767,7 @@
         <v>378</v>
       </c>
       <c r="D279" s="13">
-        <v>37740.172973148081</v>
+        <v>37740.172953050598</v>
       </c>
       <c r="E279" s="13">
         <v>99947.811107758622</v>
@@ -31787,7 +31787,7 @@
         <v>378</v>
       </c>
       <c r="D280" s="13">
-        <v>49521.931821024991</v>
+        <v>49521.931740505679</v>
       </c>
       <c r="E280" s="13">
         <v>99947.811107758622</v>
@@ -31807,7 +31807,7 @@
         <v>378</v>
       </c>
       <c r="D281" s="13">
-        <v>41374.994743593707</v>
+        <v>41374.994698407245</v>
       </c>
       <c r="E281" s="13">
         <v>99947.811107758622</v>
@@ -31827,7 +31827,7 @@
         <v>378</v>
       </c>
       <c r="D282" s="13">
-        <v>38463.310713455059</v>
+        <v>38463.310659785544</v>
       </c>
       <c r="E282" s="13">
         <v>99947.811107758622</v>
@@ -31847,7 +31847,7 @@
         <v>378</v>
       </c>
       <c r="D283" s="13">
-        <v>41112.373044003616</v>
+        <v>41112.373081952988</v>
       </c>
       <c r="E283" s="13">
         <v>99947.811107758622</v>
@@ -32127,7 +32127,7 @@
         <v>378</v>
       </c>
       <c r="D297" s="13">
-        <v>951.07368186447604</v>
+        <v>951.07368134617514</v>
       </c>
       <c r="E297" s="13">
         <v>99824.034770780301</v>
@@ -32367,7 +32367,7 @@
         <v>378</v>
       </c>
       <c r="D309" s="13">
-        <v>951.07368186447604</v>
+        <v>951.07368134617514</v>
       </c>
       <c r="E309" s="13">
         <v>99824.034770780301</v>
@@ -32447,7 +32447,7 @@
         <v>378</v>
       </c>
       <c r="D313" s="13">
-        <v>59499.506946216839</v>
+        <v>59499.506940682026</v>
       </c>
       <c r="E313" s="13">
         <v>99824.034770780301</v>
@@ -32467,7 +32467,7 @@
         <v>378</v>
       </c>
       <c r="D314" s="13">
-        <v>53650.74774956725</v>
+        <v>53650.747858444563</v>
       </c>
       <c r="E314" s="13">
         <v>99824.034770780301</v>
@@ -32487,7 +32487,7 @@
         <v>378</v>
       </c>
       <c r="D315" s="13">
-        <v>47378.392287122711</v>
+        <v>47378.392273023288</v>
       </c>
       <c r="E315" s="13">
         <v>99824.034770780301</v>
@@ -32507,7 +32507,7 @@
         <v>378</v>
       </c>
       <c r="D316" s="13">
-        <v>62599.27397272348</v>
+        <v>62599.273932027725</v>
       </c>
       <c r="E316" s="13">
         <v>99824.034770780301</v>
@@ -32527,7 +32527,7 @@
         <v>378</v>
       </c>
       <c r="D317" s="13">
-        <v>50478.159243127178</v>
+        <v>50478.159264368987</v>
       </c>
       <c r="E317" s="13">
         <v>99824.034770780301</v>
@@ -32547,7 +32547,7 @@
         <v>378</v>
       </c>
       <c r="D318" s="13">
-        <v>46590.054281706471</v>
+        <v>46590.054361301867</v>
       </c>
       <c r="E318" s="13">
         <v>99824.034770780301</v>
@@ -32567,7 +32567,7 @@
         <v>378</v>
       </c>
       <c r="D319" s="13">
-        <v>49231.887524357953</v>
+        <v>49231.887570747436</v>
       </c>
       <c r="E319" s="13">
         <v>99824.034770780301</v>
@@ -32827,7 +32827,7 @@
         <v>378</v>
       </c>
       <c r="D332" s="13">
-        <v>176.47329059086482</v>
+        <v>176.47329059086479</v>
       </c>
       <c r="E332" s="13">
         <v>100260.39175218702</v>
@@ -32847,7 +32847,7 @@
         <v>378</v>
       </c>
       <c r="D333" s="13">
-        <v>938.13810211769328</v>
+        <v>938.13810080810106</v>
       </c>
       <c r="E333" s="13">
         <v>100260.39175218702</v>
@@ -33087,7 +33087,7 @@
         <v>378</v>
       </c>
       <c r="D345" s="13">
-        <v>938.13810211769328</v>
+        <v>938.13810080810106</v>
       </c>
       <c r="E345" s="13">
         <v>100260.39175218702</v>
@@ -33167,7 +33167,7 @@
         <v>378</v>
       </c>
       <c r="D349" s="13">
-        <v>109707.98148515768</v>
+        <v>109707.98133371885</v>
       </c>
       <c r="E349" s="13">
         <v>100260.39175218702</v>
@@ -33187,7 +33187,7 @@
         <v>378</v>
       </c>
       <c r="D350" s="13">
-        <v>95761.751069302481</v>
+        <v>95761.751079426816</v>
       </c>
       <c r="E350" s="13">
         <v>100260.39175218702</v>
@@ -33207,7 +33207,7 @@
         <v>378</v>
       </c>
       <c r="D351" s="13">
-        <v>83950.05594348842</v>
+        <v>83950.056016296701</v>
       </c>
       <c r="E351" s="13">
         <v>100260.39175218702</v>
@@ -33227,7 +33227,7 @@
         <v>378</v>
       </c>
       <c r="D352" s="13">
-        <v>112347.98977346366</v>
+        <v>112347.98960337471</v>
       </c>
       <c r="E352" s="13">
         <v>100260.39175218702</v>
@@ -33247,7 +33247,7 @@
         <v>378</v>
       </c>
       <c r="D353" s="13">
-        <v>86590.064175048334</v>
+        <v>86590.064285952569</v>
       </c>
       <c r="E353" s="13">
         <v>100260.39175218702</v>
@@ -33267,7 +33267,7 @@
         <v>378</v>
       </c>
       <c r="D354" s="13">
-        <v>80359.501472963864</v>
+        <v>80359.501561709651</v>
       </c>
       <c r="E354" s="13">
         <v>100260.39175218702</v>
@@ -33287,7 +33287,7 @@
         <v>378</v>
       </c>
       <c r="D355" s="13">
-        <v>83095.767929175578</v>
+        <v>83095.768138245723</v>
       </c>
       <c r="E355" s="13">
         <v>100260.39175218702</v>
@@ -34437,7 +34437,7 @@
         <v>149</v>
       </c>
       <c r="D72" s="13">
-        <v>0.32635525530948556</v>
+        <v>0.32651812854804341</v>
       </c>
     </row>
     <row r="73">
@@ -34941,7 +34941,7 @@
         <v>149</v>
       </c>
       <c r="D108" s="13">
-        <v>0.35396611307761244</v>
+        <v>0.35337871164049528</v>
       </c>
     </row>
     <row r="109">
@@ -38497,7 +38497,7 @@
         <v>149</v>
       </c>
       <c r="D362" s="13">
-        <v>0.46088429444393814</v>
+        <v>0.46183137721612061</v>
       </c>
     </row>
     <row r="363">
@@ -39001,7 +39001,7 @@
         <v>149</v>
       </c>
       <c r="D398" s="13">
-        <v>0.51570211258427379</v>
+        <v>0.51760124616362779</v>
       </c>
     </row>
     <row r="399">

</xml_diff>

<commit_message>
MOdifying excel file with all necesary objects
</commit_message>
<xml_diff>
--- a/03.Tool/Example_FiscalSim.xlsx
+++ b/03.Tool/Example_FiscalSim.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/dvalderramagonza_worldbank_org/Documents/Example_FiscalSim/03.Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{677CB6D6-9ADB-4CCD-A457-B7E26AE541CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E9D6E86-AA35-4AD9-9519-9DF7EF5CEE74}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{677CB6D6-9ADB-4CCD-A457-B7E26AE541CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08765EC9-5738-4642-815C-B88244E87E3E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3722" uniqueCount="1484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3723" uniqueCount="1485">
   <si>
     <t>Bracket</t>
   </si>
@@ -4536,7 +4536,10 @@
     <t>max number of eligible children</t>
   </si>
   <si>
-    <t>VAT_exempt_share</t>
+    <t>VAT_exempt_share_PY</t>
+  </si>
+  <si>
+    <t>VAT_exempt_share_SY</t>
   </si>
 </sst>
 </file>
@@ -24479,9 +24482,7 @@
   </sheetPr>
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -39144,14 +39145,14 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="J44" sqref="J44"/>
       <selection pane="topRight" activeCell="J44" sqref="J44"/>
       <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
-      <selection pane="bottomRight" activeCell="W3" sqref="W3"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2:U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39160,11 +39161,11 @@
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1099</v>
       </c>
@@ -39226,16 +39227,19 @@
         <v>1119</v>
       </c>
       <c r="U1" t="s">
+        <v>1484</v>
+      </c>
+      <c r="V1" t="s">
         <v>1101</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>1120</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>1483</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -39295,18 +39299,21 @@
       </c>
       <c r="T2" s="195"/>
       <c r="U2" s="129">
+        <v>0.2</v>
+      </c>
+      <c r="V2" s="129">
         <f>Parameters!$C$43</f>
         <v>0.18</v>
       </c>
-      <c r="V2" s="195">
+      <c r="W2" s="195">
         <f>T2</f>
         <v>0</v>
       </c>
-      <c r="W2" s="129">
+      <c r="X2" s="129">
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -39366,18 +39373,21 @@
       </c>
       <c r="T3" s="195"/>
       <c r="U3" s="129">
+        <v>0.6</v>
+      </c>
+      <c r="V3" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="V3" s="195">
-        <f t="shared" ref="V3:V17" si="0">T3</f>
+      <c r="W3" s="195">
+        <f t="shared" ref="W3:W17" si="0">T3</f>
         <v>0</v>
       </c>
-      <c r="W3" s="129">
+      <c r="X3" s="129">
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -39437,18 +39447,21 @@
       </c>
       <c r="T4" s="195"/>
       <c r="U4" s="129">
+        <v>0.8</v>
+      </c>
+      <c r="V4" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="V4" s="195">
+      <c r="W4" s="195">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W4" s="129">
+      <c r="X4" s="129">
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -39507,17 +39520,18 @@
         <v>0</v>
       </c>
       <c r="T5" s="195"/>
-      <c r="U5" s="129">
+      <c r="U5" s="129"/>
+      <c r="V5" s="129">
         <f>Parameters!$C$44</f>
         <v>0</v>
       </c>
-      <c r="V5" s="195">
+      <c r="W5" s="195">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W5" s="129"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" s="129"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -39576,17 +39590,18 @@
         <v>0.25</v>
       </c>
       <c r="T6" s="195"/>
-      <c r="U6" s="129">
+      <c r="U6" s="129"/>
+      <c r="V6" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="V6" s="195">
+      <c r="W6" s="195">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W6" s="129"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" s="129"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -39645,17 +39660,18 @@
         <v>0.25</v>
       </c>
       <c r="T7" s="195"/>
-      <c r="U7" s="129">
+      <c r="U7" s="129"/>
+      <c r="V7" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="V7" s="195">
+      <c r="W7" s="195">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W7" s="129"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7" s="129"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -39714,16 +39730,19 @@
       <c r="T8" s="195">
         <v>1</v>
       </c>
-      <c r="U8" s="129"/>
-      <c r="V8" s="195">
+      <c r="U8" s="129">
+        <v>1</v>
+      </c>
+      <c r="V8" s="129"/>
+      <c r="W8" s="195">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W8" s="129">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -39782,17 +39801,18 @@
         <v>0</v>
       </c>
       <c r="T9" s="195"/>
-      <c r="U9" s="129">
+      <c r="U9" s="129"/>
+      <c r="V9" s="129">
         <f>Parameters!$C$44</f>
         <v>0</v>
       </c>
-      <c r="V9" s="195">
+      <c r="W9" s="195">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W9" s="129"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" s="129"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -39851,17 +39871,18 @@
         <v>0.25</v>
       </c>
       <c r="T10" s="195"/>
-      <c r="U10" s="129">
+      <c r="U10" s="129"/>
+      <c r="V10" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="V10" s="195">
+      <c r="W10" s="195">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W10" s="129"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" s="129"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -39920,16 +39941,19 @@
       <c r="T11" s="195">
         <v>1</v>
       </c>
-      <c r="U11" s="129"/>
-      <c r="V11" s="195">
+      <c r="U11" s="129">
+        <v>0.4</v>
+      </c>
+      <c r="V11" s="129"/>
+      <c r="W11" s="195">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W11" s="129">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X11" s="129">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -39988,16 +40012,19 @@
       <c r="T12" s="195">
         <v>1</v>
       </c>
-      <c r="U12" s="129"/>
-      <c r="V12" s="195">
+      <c r="U12" s="129">
+        <v>0.4</v>
+      </c>
+      <c r="V12" s="129"/>
+      <c r="W12" s="195">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W12" s="129">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12" s="129">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -40056,16 +40083,19 @@
       <c r="T13" s="195">
         <v>1</v>
       </c>
-      <c r="U13" s="129"/>
-      <c r="V13" s="195">
+      <c r="U13" s="129">
+        <v>0.4</v>
+      </c>
+      <c r="V13" s="129"/>
+      <c r="W13" s="195">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W13" s="129">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X13" s="129">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -40124,16 +40154,19 @@
       <c r="T14" s="195">
         <v>1</v>
       </c>
-      <c r="U14" s="129"/>
-      <c r="V14" s="195">
+      <c r="U14" s="129">
+        <v>0.8</v>
+      </c>
+      <c r="V14" s="129"/>
+      <c r="W14" s="195">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W14" s="129">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X14" s="129">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -40192,16 +40225,19 @@
       <c r="T15" s="195">
         <v>1</v>
       </c>
-      <c r="U15" s="129"/>
-      <c r="V15" s="195">
+      <c r="U15" s="129">
+        <v>0.8</v>
+      </c>
+      <c r="V15" s="129"/>
+      <c r="W15" s="195">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W15" s="129">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X15" s="129">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -40260,16 +40296,19 @@
       <c r="T16" s="195">
         <v>1</v>
       </c>
-      <c r="U16" s="129"/>
-      <c r="V16" s="195">
+      <c r="U16" s="129">
+        <v>0.8</v>
+      </c>
+      <c r="V16" s="129"/>
+      <c r="W16" s="195">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W16" s="129">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X16" s="129">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -40328,13 +40367,16 @@
       <c r="T17" s="195">
         <v>1</v>
       </c>
-      <c r="U17" s="129"/>
-      <c r="V17" s="195">
+      <c r="U17" s="129">
+        <v>0.8</v>
+      </c>
+      <c r="V17" s="129"/>
+      <c r="W17" s="195">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W17" s="129">
-        <v>0.5</v>
+      <c r="X17" s="129">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -48274,6 +48316,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3F2126381553441AAB919CB53585984" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f1b497080c7a9ebe3361009889ddd89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ac8e30ca-65e9-4041-b86a-4d1b6d416c33" xmlns:ns4="fb6f0dd5-0349-47c8-82f6-4423e71a7ac1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a52065183d7b0fe9b0b93a9043295234" ns3:_="" ns4:_="">
     <xsd:import namespace="ac8e30ca-65e9-4041-b86a-4d1b6d416c33"/>
@@ -48496,15 +48547,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -48512,6 +48554,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D121BB-2F17-4CB9-A6EB-F21D520CE0DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{896EEE12-401D-4484-A123-4E3419FF9B2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -48530,14 +48580,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D121BB-2F17-4CB9-A6EB-F21D520CE0DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{688B2FF8-EC2C-43B6-830F-CB3A5682666A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Auto stash before merge of "vat_changes" and "origin/main"
</commit_message>
<xml_diff>
--- a/03.Tool/Example_FiscalSim.xlsx
+++ b/03.Tool/Example_FiscalSim.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/dvalderramagonza_worldbank_org/Documents/Example_FiscalSim/03.Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{677CB6D6-9ADB-4CCD-A457-B7E26AE541CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08765EC9-5738-4642-815C-B88244E87E3E}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{677CB6D6-9ADB-4CCD-A457-B7E26AE541CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DF3EF3E-8E47-4A13-A4C9-A6BA833307C1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -4546,11 +4546,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -5209,7 +5210,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="270">
+  <cellXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5791,6 +5792,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -14082,8 +14086,8 @@
   <dimension ref="A2:E67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24482,7 +24486,9 @@
   </sheetPr>
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -39147,12 +39153,12 @@
   </sheetPr>
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="J44" sqref="J44"/>
       <selection pane="topRight" activeCell="J44" sqref="J44"/>
       <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
-      <selection pane="bottomRight" activeCell="U2" sqref="U2:U17"/>
+      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39161,8 +39167,9 @@
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" customWidth="1"/>
     <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -39297,7 +39304,9 @@
       <c r="S2" s="129">
         <v>0.18</v>
       </c>
-      <c r="T2" s="195"/>
+      <c r="T2" s="195">
+        <v>0</v>
+      </c>
       <c r="U2" s="129">
         <v>0.2</v>
       </c>
@@ -39305,7 +39314,7 @@
         <f>Parameters!$C$43</f>
         <v>0.18</v>
       </c>
-      <c r="W2" s="195">
+      <c r="W2" s="243">
         <f>T2</f>
         <v>0</v>
       </c>
@@ -39371,21 +39380,19 @@
       <c r="S3" s="129">
         <v>0.25</v>
       </c>
-      <c r="T3" s="195"/>
-      <c r="U3" s="129">
-        <v>0.6</v>
-      </c>
+      <c r="T3" s="195">
+        <v>0</v>
+      </c>
+      <c r="U3" s="129"/>
       <c r="V3" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="W3" s="195">
-        <f t="shared" ref="W3:W17" si="0">T3</f>
+      <c r="W3" s="243">
+        <f t="shared" ref="W3:W16" si="0">T3</f>
         <v>0</v>
       </c>
-      <c r="X3" s="129">
-        <v>0.6</v>
-      </c>
+      <c r="X3" s="129"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -39445,21 +39452,19 @@
       <c r="S4" s="129">
         <v>0.25</v>
       </c>
-      <c r="T4" s="195"/>
-      <c r="U4" s="129">
-        <v>0.8</v>
-      </c>
+      <c r="T4" s="195">
+        <v>0</v>
+      </c>
+      <c r="U4" s="129"/>
       <c r="V4" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="W4" s="195">
+      <c r="W4" s="243">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X4" s="129">
-        <v>0.8</v>
-      </c>
+      <c r="X4" s="129"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -39519,13 +39524,15 @@
       <c r="S5" s="129">
         <v>0</v>
       </c>
-      <c r="T5" s="195"/>
+      <c r="T5" s="195">
+        <v>0</v>
+      </c>
       <c r="U5" s="129"/>
       <c r="V5" s="129">
         <f>Parameters!$C$44</f>
         <v>0</v>
       </c>
-      <c r="W5" s="195">
+      <c r="W5" s="243">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -39589,13 +39596,15 @@
       <c r="S6" s="129">
         <v>0.25</v>
       </c>
-      <c r="T6" s="195"/>
+      <c r="T6" s="195">
+        <v>0</v>
+      </c>
       <c r="U6" s="129"/>
       <c r="V6" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="W6" s="195">
+      <c r="W6" s="243">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -39659,13 +39668,15 @@
       <c r="S7" s="129">
         <v>0.25</v>
       </c>
-      <c r="T7" s="195"/>
+      <c r="T7" s="195">
+        <v>0</v>
+      </c>
       <c r="U7" s="129"/>
       <c r="V7" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="W7" s="195">
+      <c r="W7" s="243">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -39734,7 +39745,7 @@
         <v>1</v>
       </c>
       <c r="V8" s="129"/>
-      <c r="W8" s="195">
+      <c r="W8" s="243">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -39800,13 +39811,15 @@
       <c r="S9" s="129">
         <v>0</v>
       </c>
-      <c r="T9" s="195"/>
+      <c r="T9" s="195">
+        <v>0</v>
+      </c>
       <c r="U9" s="129"/>
       <c r="V9" s="129">
         <f>Parameters!$C$44</f>
         <v>0</v>
       </c>
-      <c r="W9" s="195">
+      <c r="W9" s="243">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -39870,13 +39883,15 @@
       <c r="S10" s="129">
         <v>0.25</v>
       </c>
-      <c r="T10" s="195"/>
+      <c r="T10" s="195">
+        <v>0</v>
+      </c>
       <c r="U10" s="129"/>
       <c r="V10" s="129">
         <f>Parameters!$C$42</f>
         <v>0.25</v>
       </c>
-      <c r="W10" s="195">
+      <c r="W10" s="243">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -39942,15 +39957,18 @@
         <v>1</v>
       </c>
       <c r="U11" s="129">
-        <v>0.4</v>
-      </c>
-      <c r="V11" s="129"/>
-      <c r="W11" s="195">
+        <v>0.2</v>
+      </c>
+      <c r="V11" s="129">
+        <f>Parameters!$C$42</f>
+        <v>0.25</v>
+      </c>
+      <c r="W11" s="243">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X11" s="129">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -40013,15 +40031,18 @@
         <v>1</v>
       </c>
       <c r="U12" s="129">
-        <v>0.4</v>
-      </c>
-      <c r="V12" s="129"/>
-      <c r="W12" s="195">
+        <v>0.5</v>
+      </c>
+      <c r="V12" s="129">
+        <f>Parameters!$C$42</f>
+        <v>0.25</v>
+      </c>
+      <c r="W12" s="243">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X12" s="129">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -40084,15 +40105,18 @@
         <v>1</v>
       </c>
       <c r="U13" s="129">
-        <v>0.4</v>
-      </c>
-      <c r="V13" s="129"/>
-      <c r="W13" s="195">
+        <v>0.5</v>
+      </c>
+      <c r="V13" s="129">
+        <f>Parameters!$C$42</f>
+        <v>0.25</v>
+      </c>
+      <c r="W13" s="243">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X13" s="129">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -40155,10 +40179,13 @@
         <v>1</v>
       </c>
       <c r="U14" s="129">
-        <v>0.8</v>
-      </c>
-      <c r="V14" s="129"/>
-      <c r="W14" s="195">
+        <v>0.5</v>
+      </c>
+      <c r="V14" s="129">
+        <f>Parameters!$C$42</f>
+        <v>0.25</v>
+      </c>
+      <c r="W14" s="243">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -40226,10 +40253,13 @@
         <v>1</v>
       </c>
       <c r="U15" s="129">
-        <v>0.8</v>
-      </c>
-      <c r="V15" s="129"/>
-      <c r="W15" s="195">
+        <v>0.5</v>
+      </c>
+      <c r="V15" s="129">
+        <f>Parameters!$C$42</f>
+        <v>0.25</v>
+      </c>
+      <c r="W15" s="243">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -40297,10 +40327,13 @@
         <v>1</v>
       </c>
       <c r="U16" s="129">
-        <v>0.8</v>
-      </c>
-      <c r="V16" s="129"/>
-      <c r="W16" s="195">
+        <v>0.5</v>
+      </c>
+      <c r="V16" s="129">
+        <f>Parameters!$C$42</f>
+        <v>0.25</v>
+      </c>
+      <c r="W16" s="243">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -40368,11 +40401,14 @@
         <v>1</v>
       </c>
       <c r="U17" s="129">
-        <v>0.8</v>
-      </c>
-      <c r="V17" s="129"/>
-      <c r="W17" s="195">
-        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="V17" s="129">
+        <f>Parameters!$C$42</f>
+        <v>0.25</v>
+      </c>
+      <c r="W17" s="243">
+        <f>T17</f>
         <v>1</v>
       </c>
       <c r="X17" s="129">
@@ -40451,24 +40487,24 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="O3" s="4"/>
-      <c r="Q3" s="243"/>
-      <c r="R3" s="243"/>
-      <c r="S3" s="243"/>
-      <c r="T3" s="243"/>
-      <c r="U3" s="243"/>
-      <c r="V3" s="243"/>
+      <c r="Q3" s="244"/>
+      <c r="R3" s="244"/>
+      <c r="S3" s="244"/>
+      <c r="T3" s="244"/>
+      <c r="U3" s="244"/>
+      <c r="V3" s="244"/>
       <c r="AK3"/>
     </row>
     <row r="4" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
-      <c r="B4" s="244" t="s">
+      <c r="B4" s="245" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="245"/>
-      <c r="D4" s="245"/>
-      <c r="E4" s="245"/>
-      <c r="F4" s="245"/>
-      <c r="G4" s="246"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="246"/>
+      <c r="G4" s="247"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="O4" s="4"/>
@@ -41215,12 +41251,12 @@
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
       <c r="P3" s="4"/>
-      <c r="R3" s="243"/>
-      <c r="S3" s="243"/>
-      <c r="T3" s="243"/>
-      <c r="U3" s="243"/>
-      <c r="V3" s="243"/>
-      <c r="W3" s="243"/>
+      <c r="R3" s="244"/>
+      <c r="S3" s="244"/>
+      <c r="T3" s="244"/>
+      <c r="U3" s="244"/>
+      <c r="V3" s="244"/>
+      <c r="W3" s="244"/>
       <c r="AL3"/>
     </row>
     <row r="4" spans="1:38" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -42248,18 +42284,18 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
-      <c r="X4" s="247" t="s">
+      <c r="X4" s="248" t="s">
         <v>36</v>
       </c>
-      <c r="Y4" s="248"/>
-      <c r="Z4" s="248"/>
-      <c r="AA4" s="248"/>
-      <c r="AB4" s="248"/>
-      <c r="AC4" s="248"/>
-      <c r="AD4" s="248"/>
-      <c r="AE4" s="248"/>
-      <c r="AF4" s="248"/>
-      <c r="AG4" s="249"/>
+      <c r="Y4" s="249"/>
+      <c r="Z4" s="249"/>
+      <c r="AA4" s="249"/>
+      <c r="AB4" s="249"/>
+      <c r="AC4" s="249"/>
+      <c r="AD4" s="249"/>
+      <c r="AE4" s="249"/>
+      <c r="AF4" s="249"/>
+      <c r="AG4" s="250"/>
     </row>
     <row r="5" spans="1:61" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="43"/>
@@ -44302,20 +44338,20 @@
       <c r="B2">
         <v>34626.576694199313</v>
       </c>
-      <c r="E2" s="250" t="s">
+      <c r="E2" s="251" t="s">
         <v>778</v>
       </c>
-      <c r="F2" s="251"/>
-      <c r="G2" s="251"/>
-      <c r="H2" s="251"/>
-      <c r="I2" s="251"/>
-      <c r="J2" s="251"/>
-      <c r="K2" s="251"/>
-      <c r="L2" s="251"/>
-      <c r="M2" s="251"/>
-      <c r="N2" s="251"/>
-      <c r="O2" s="251"/>
-      <c r="P2" s="252"/>
+      <c r="F2" s="252"/>
+      <c r="G2" s="252"/>
+      <c r="H2" s="252"/>
+      <c r="I2" s="252"/>
+      <c r="J2" s="252"/>
+      <c r="K2" s="252"/>
+      <c r="L2" s="252"/>
+      <c r="M2" s="252"/>
+      <c r="N2" s="252"/>
+      <c r="O2" s="252"/>
+      <c r="P2" s="253"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
@@ -44344,10 +44380,10 @@
       <c r="L3" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="253" t="s">
+      <c r="M3" s="254" t="s">
         <v>784</v>
       </c>
-      <c r="N3" s="253"/>
+      <c r="N3" s="254"/>
       <c r="O3" s="113" t="s">
         <v>16</v>
       </c>
@@ -46103,24 +46139,24 @@
   <sheetData>
     <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="4:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D5" s="254" t="s">
+      <c r="D5" s="255" t="s">
         <v>795</v>
       </c>
-      <c r="E5" s="255"/>
-      <c r="F5" s="255"/>
-      <c r="G5" s="255"/>
-      <c r="H5" s="256"/>
+      <c r="E5" s="256"/>
+      <c r="F5" s="256"/>
+      <c r="G5" s="256"/>
+      <c r="H5" s="257"/>
     </row>
     <row r="6" spans="4:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D6" s="134" t="s">
         <v>796</v>
       </c>
       <c r="E6" s="135"/>
-      <c r="F6" s="257" t="s">
+      <c r="F6" s="258" t="s">
         <v>797</v>
       </c>
-      <c r="G6" s="257"/>
-      <c r="H6" s="258"/>
+      <c r="G6" s="258"/>
+      <c r="H6" s="259"/>
     </row>
     <row r="7" spans="4:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D7" s="136"/>
@@ -46188,21 +46224,21 @@
     </row>
     <row r="13" spans="4:15" ht="13.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="259" t="s">
+      <c r="D14" s="260" t="s">
         <v>803</v>
       </c>
-      <c r="E14" s="260"/>
-      <c r="F14" s="261"/>
-      <c r="H14" s="259" t="s">
+      <c r="E14" s="261"/>
+      <c r="F14" s="262"/>
+      <c r="H14" s="260" t="s">
         <v>804</v>
       </c>
-      <c r="I14" s="260"/>
-      <c r="J14" s="261"/>
-      <c r="M14" s="262" t="s">
+      <c r="I14" s="261"/>
+      <c r="J14" s="262"/>
+      <c r="M14" s="263" t="s">
         <v>805</v>
       </c>
-      <c r="N14" s="263"/>
-      <c r="O14" s="264"/>
+      <c r="N14" s="264"/>
+      <c r="O14" s="265"/>
     </row>
     <row r="15" spans="4:15" s="23" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="130"/>
@@ -46699,13 +46735,13 @@
       <c r="B2" s="168">
         <v>34626.576694199313</v>
       </c>
-      <c r="H2" s="265" t="s">
+      <c r="H2" s="266" t="s">
         <v>1088</v>
       </c>
-      <c r="I2" s="266"/>
-      <c r="J2" s="266"/>
-      <c r="K2" s="266"/>
-      <c r="L2" s="267"/>
+      <c r="I2" s="267"/>
+      <c r="J2" s="267"/>
+      <c r="K2" s="267"/>
+      <c r="L2" s="268"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="168" t="str">
@@ -46719,10 +46755,10 @@
       <c r="J3" s="177" t="s">
         <v>1089</v>
       </c>
-      <c r="K3" s="268" t="s">
+      <c r="K3" s="269" t="s">
         <v>1090</v>
       </c>
-      <c r="L3" s="269"/>
+      <c r="L3" s="270"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="168" t="str">
@@ -48316,15 +48352,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3F2126381553441AAB919CB53585984" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f1b497080c7a9ebe3361009889ddd89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ac8e30ca-65e9-4041-b86a-4d1b6d416c33" xmlns:ns4="fb6f0dd5-0349-47c8-82f6-4423e71a7ac1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a52065183d7b0fe9b0b93a9043295234" ns3:_="" ns4:_="">
     <xsd:import namespace="ac8e30ca-65e9-4041-b86a-4d1b6d416c33"/>
@@ -48547,6 +48574,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -48554,14 +48590,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D121BB-2F17-4CB9-A6EB-F21D520CE0DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{896EEE12-401D-4484-A123-4E3419FF9B2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -48580,6 +48608,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D121BB-2F17-4CB9-A6EB-F21D520CE0DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{688B2FF8-EC2C-43B6-830F-CB3A5682666A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
merging all files to main
</commit_message>
<xml_diff>
--- a/03.Tool/Example_FiscalSim.xlsx
+++ b/03.Tool/Example_FiscalSim.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="10829" uniqueCount="2022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="14299" uniqueCount="2022">
   <si>
     <t>Bracket</t>
   </si>
@@ -17734,7 +17734,7 @@
         <v>-203.518850710631</v>
       </c>
       <c r="AE6" s="64">
-        <v>-13.62658662456351</v>
+        <v>-13.62658662456352</v>
       </c>
       <c r="AF6" s="64">
         <v>32.23618891149637</v>
@@ -19116,7 +19116,7 @@
         <v>6.487402886297008</v>
       </c>
       <c r="AH17" s="64">
-        <v>6.041287857945126</v>
+        <v>6.041287857945125</v>
       </c>
       <c r="AI17" s="64">
         <v>3.604304436742737</v>
@@ -20825,7 +20825,7 @@
         <v>-213.408292786445</v>
       </c>
       <c r="N31" s="64">
-        <v>26.39312458358597</v>
+        <v>26.39312458358598</v>
       </c>
       <c r="O31" s="64">
         <v>105.6331513178878</v>
@@ -21853,7 +21853,7 @@
         <v>-969.4662503529736</v>
       </c>
       <c r="AE39" s="64">
-        <v>-70.6527951610056</v>
+        <v>-70.65279516100559</v>
       </c>
       <c r="AF39" s="64">
         <v>97.07688119459668</v>
@@ -21976,7 +21976,7 @@
         <v>210.3747342958241</v>
       </c>
       <c r="AB40" s="64">
-        <v>98.97972670544188</v>
+        <v>98.97972670544186</v>
       </c>
       <c r="AC40" s="64">
         <v>31.29092663388508</v>
@@ -34648,7 +34648,7 @@
         <v>891</v>
       </c>
       <c r="D312" s="13">
-        <v>361.9998384268768</v>
+        <v>361.9998384268767</v>
       </c>
       <c r="E312" s="13">
         <v>99824.0347707803</v>

</xml_diff>